<commit_message>
se le quito las migajas en nuevo pedido
</commit_message>
<xml_diff>
--- a/database/BD/backup/precios.xlsx
+++ b/database/BD/backup/precios.xlsx
@@ -871,9 +871,6 @@
     <t>Llave de paso 1/2" - simbal</t>
   </si>
   <si>
-    <t>Ladrillo pandereta (hasta 250 unidades)</t>
-  </si>
-  <si>
     <t>Codo bronce de 1/2"</t>
   </si>
   <si>
@@ -890,6 +887,9 @@
   </si>
   <si>
     <t>Liston 2.5 metros</t>
+  </si>
+  <si>
+    <t>Ladrillo pandereta (unidad)</t>
   </si>
 </sst>
 </file>
@@ -3126,8 +3126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="D124" sqref="D124"/>
+    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="C125" sqref="C125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4326,7 +4326,7 @@
         <v>241</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D29" s="3">
         <v>4.5</v>
@@ -8411,24 +8411,24 @@
         <v>241</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D124" s="3">
-        <v>0.44</v>
+        <v>0.5</v>
       </c>
       <c r="G124" t="s">
         <v>267</v>
       </c>
       <c r="H124" t="str">
         <f t="shared" ref="H124" si="16">C124</f>
-        <v>Ladrillo pandereta (hasta 250 unidades)</v>
+        <v>Ladrillo pandereta (unidad)</v>
       </c>
       <c r="I124" s="7" t="s">
         <v>266</v>
       </c>
       <c r="J124" s="3">
         <f t="shared" ref="J124" si="17">D124</f>
-        <v>0.44</v>
+        <v>0.5</v>
       </c>
       <c r="K124" t="s">
         <v>269</v>
@@ -8442,7 +8442,7 @@
       </c>
       <c r="N124" t="str">
         <f t="shared" ref="N124" si="19">CONCATENATE(G124,H124,I124,J124,K124,L124,M124)</f>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Ladrillo pandereta (hasta 250 unidades)', 0.44, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Ladrillo pandereta (unidad)', 0.5, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.25">
@@ -8497,7 +8497,7 @@
         <v>249</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D126" s="3">
         <v>3.5</v>
@@ -8540,7 +8540,7 @@
         <v>241</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D127" s="3">
         <v>8</v>
@@ -8549,14 +8549,14 @@
         <v>267</v>
       </c>
       <c r="H127" t="str">
-        <f t="shared" ref="H127:H128" si="28">C127</f>
+        <f t="shared" ref="H127" si="28">C127</f>
         <v>Parante 3 metros</v>
       </c>
       <c r="I127" s="7" t="s">
         <v>266</v>
       </c>
       <c r="J127" s="3">
-        <f t="shared" ref="J127:J129" si="29">D127</f>
+        <f t="shared" ref="J127" si="29">D127</f>
         <v>8</v>
       </c>
       <c r="K127" t="s">
@@ -8583,7 +8583,7 @@
         <v>241</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D128" s="3">
         <v>7</v>
@@ -8626,7 +8626,7 @@
         <v>241</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D129" s="3">
         <v>4.5</v>
@@ -8669,7 +8669,7 @@
         <v>241</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D130" s="3">
         <v>4</v>

</xml_diff>

<commit_message>
busqueda de items mejorado!
</commit_message>
<xml_diff>
--- a/database/BD/backup/precios.xlsx
+++ b/database/BD/backup/precios.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="288">
   <si>
     <t>Tubos</t>
   </si>
@@ -890,6 +890,9 @@
   </si>
   <si>
     <t>Ladrillo pandereta (unidad)</t>
+  </si>
+  <si>
+    <t>Ladrillo de techo 12 x 30 (unidad)</t>
   </si>
 </sst>
 </file>
@@ -3124,10 +3127,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N130"/>
+  <dimension ref="A1:N131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="C125" sqref="C125"/>
+    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
+      <selection activeCell="C131" sqref="C131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8599,7 +8602,7 @@
         <v>266</v>
       </c>
       <c r="J128" s="3">
-        <f t="shared" ref="J128:J130" si="33">D128</f>
+        <f t="shared" ref="J128:J131" si="33">D128</f>
         <v>7</v>
       </c>
       <c r="K128" t="s">
@@ -8701,6 +8704,49 @@
       <c r="N130" t="str">
         <f t="shared" si="35"/>
         <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Liston 2.5 metros', 4, 'Activo', 0, 0, 3 ) ; </v>
+      </c>
+    </row>
+    <row r="131" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <f>VLOOKUP(B131,'Maestra de unidades'!$B:$C,2,0)</f>
+        <v>3</v>
+      </c>
+      <c r="B131" t="s">
+        <v>241</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="D131" s="3">
+        <v>2.1</v>
+      </c>
+      <c r="G131" t="s">
+        <v>267</v>
+      </c>
+      <c r="H131" t="str">
+        <f t="shared" ref="H131" si="36">C131</f>
+        <v>Ladrillo de techo 12 x 30 (unidad)</v>
+      </c>
+      <c r="I131" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="J131" s="3">
+        <f t="shared" ref="J131" si="37">D131</f>
+        <v>2.1</v>
+      </c>
+      <c r="K131" t="s">
+        <v>269</v>
+      </c>
+      <c r="L131">
+        <f t="shared" ref="L131" si="38">A131</f>
+        <v>3</v>
+      </c>
+      <c r="M131" t="s">
+        <v>268</v>
+      </c>
+      <c r="N131" t="str">
+        <f t="shared" ref="N131" si="39">CONCATENATE(G131,H131,I131,J131,K131,L131,M131)</f>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Ladrillo de techo 12 x 30 (unidad)', 2.1, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se agrego la posibilidad de ser proforma
</commit_message>
<xml_diff>
--- a/database/BD/backup/precios.xlsx
+++ b/database/BD/backup/precios.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="286">
   <si>
     <t>Tubos</t>
   </si>
@@ -887,9 +887,6 @@
   </si>
   <si>
     <t>Liston 2.5 metros</t>
-  </si>
-  <si>
-    <t>Ladrillo de techo 12 x 30 (unidad)</t>
   </si>
 </sst>
 </file>
@@ -3124,10 +3121,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N130"/>
+  <dimension ref="A1:N129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="C128" sqref="C128"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="C122" sqref="C122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8658,49 +8655,6 @@
       <c r="N129" t="str">
         <f t="shared" si="31"/>
         <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Liston 2.5 metros', 4, 'Activo', 0, 0, 3 ) ; </v>
-      </c>
-    </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A130">
-        <f>VLOOKUP(B130,'Maestra de unidades'!$B:$C,2,0)</f>
-        <v>3</v>
-      </c>
-      <c r="B130" t="s">
-        <v>241</v>
-      </c>
-      <c r="C130" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="D130" s="3">
-        <v>2.1</v>
-      </c>
-      <c r="G130" t="s">
-        <v>267</v>
-      </c>
-      <c r="H130" t="str">
-        <f t="shared" ref="H130" si="32">C130</f>
-        <v>Ladrillo de techo 12 x 30 (unidad)</v>
-      </c>
-      <c r="I130" s="7" t="s">
-        <v>266</v>
-      </c>
-      <c r="J130" s="3">
-        <f t="shared" ref="J130" si="33">D130</f>
-        <v>2.1</v>
-      </c>
-      <c r="K130" t="s">
-        <v>269</v>
-      </c>
-      <c r="L130">
-        <f t="shared" ref="L130" si="34">A130</f>
-        <v>3</v>
-      </c>
-      <c r="M130" t="s">
-        <v>268</v>
-      </c>
-      <c r="N130" t="str">
-        <f t="shared" ref="N130" si="35">CONCATENATE(G130,H130,I130,J130,K130,L130,M130)</f>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Ladrillo de techo 12 x 30 (unidad)', 2.1, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
precios y nombres actualizados
</commit_message>
<xml_diff>
--- a/database/BD/backup/precios.xlsx
+++ b/database/BD/backup/precios.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="387">
   <si>
     <t>Tubos</t>
   </si>
@@ -859,9 +859,6 @@
     <t>Cemento sol tipo 1</t>
   </si>
   <si>
-    <t>Fierro de 5/8" - siderperu</t>
-  </si>
-  <si>
     <t>Rectangular</t>
   </si>
   <si>
@@ -871,22 +868,328 @@
     <t>Llave de paso 1/2" - simbal</t>
   </si>
   <si>
-    <t>Codo bronce de 1/2"</t>
-  </si>
-  <si>
     <t>Aceite 3 en 1</t>
   </si>
   <si>
-    <t>Parante 3 metros</t>
-  </si>
-  <si>
-    <t>Liston 3 metros</t>
-  </si>
-  <si>
-    <t>Parante 2.5 metros</t>
-  </si>
-  <si>
-    <t>Liston 2.5 metros</t>
+    <t>Ladrillo pandereta</t>
+  </si>
+  <si>
+    <t>Adaptador agua 1/2"</t>
+  </si>
+  <si>
+    <t>Adaptador agua 3/4"</t>
+  </si>
+  <si>
+    <t>Adaptador agua 1/2" caliente</t>
+  </si>
+  <si>
+    <t>Alambre N16</t>
+  </si>
+  <si>
+    <t>Alambre N8</t>
+  </si>
+  <si>
+    <t>Cable de luz N12</t>
+  </si>
+  <si>
+    <t>Cable de luz N14</t>
+  </si>
+  <si>
+    <t>Calamina 3.0m</t>
+  </si>
+  <si>
+    <t>Calamina 3.6m</t>
+  </si>
+  <si>
+    <t>Clavo 1y1/2"</t>
+  </si>
+  <si>
+    <t>Clavo 1"</t>
+  </si>
+  <si>
+    <t>Clavo 2"</t>
+  </si>
+  <si>
+    <t>Clavo 3"</t>
+  </si>
+  <si>
+    <t>Clavo 4"</t>
+  </si>
+  <si>
+    <t>Clavo acero 2"</t>
+  </si>
+  <si>
+    <t>Clavo acero 3"</t>
+  </si>
+  <si>
+    <t>Clavo acero 4"</t>
+  </si>
+  <si>
+    <t>Clavo calamina</t>
+  </si>
+  <si>
+    <t>Codo bronce 1/2"</t>
+  </si>
+  <si>
+    <t>Codo agua 1/2"</t>
+  </si>
+  <si>
+    <t>Codo agua 3/4" 45°</t>
+  </si>
+  <si>
+    <t>Codo agua 3/4" 90°</t>
+  </si>
+  <si>
+    <t>Codo desague 2" 45°</t>
+  </si>
+  <si>
+    <t>Codo desague 2" 90°</t>
+  </si>
+  <si>
+    <t>Codo desague 4" 45°</t>
+  </si>
+  <si>
+    <t>Codo agua caliente 1/2"</t>
+  </si>
+  <si>
+    <t>Codo desague 4" 90°</t>
+  </si>
+  <si>
+    <t>Codo desague 4"a2"</t>
+  </si>
+  <si>
+    <t>Codo luz 1"</t>
+  </si>
+  <si>
+    <t>Codo luz 3/4"</t>
+  </si>
+  <si>
+    <t>Codo galvanizado 1/2"</t>
+  </si>
+  <si>
+    <t>Disco corte fierro 14"</t>
+  </si>
+  <si>
+    <t>Disco corte fierro 4"</t>
+  </si>
+  <si>
+    <t>Disco corte fierro 7"</t>
+  </si>
+  <si>
+    <t>Disco corte fierro 9"</t>
+  </si>
+  <si>
+    <t>Disco para concreto 15" - dinamo</t>
+  </si>
+  <si>
+    <t>Disco para concreto 15" - kamasa</t>
+  </si>
+  <si>
+    <t>Disco para concreto 30" - dinamo</t>
+  </si>
+  <si>
+    <t>Disco para concreto 4" - dinamo</t>
+  </si>
+  <si>
+    <t>Disco para concreto 4" - kamasa</t>
+  </si>
+  <si>
+    <t>Fierro 1/2" - siderperu</t>
+  </si>
+  <si>
+    <t>Fierro 1/4" 6mm - siderperu</t>
+  </si>
+  <si>
+    <t>Fierro 3/4" - siderperu</t>
+  </si>
+  <si>
+    <t>Fierro 3/8" - siderperu</t>
+  </si>
+  <si>
+    <t>Fierro 5/8" - siderperu</t>
+  </si>
+  <si>
+    <t>Fierro 8mm - siderperu</t>
+  </si>
+  <si>
+    <t>Foco 27 W</t>
+  </si>
+  <si>
+    <t>Foco 32 W</t>
+  </si>
+  <si>
+    <t>Foco 42 W</t>
+  </si>
+  <si>
+    <t>Foco 85 W</t>
+  </si>
+  <si>
+    <t>Foco LED 7 W</t>
+  </si>
+  <si>
+    <t>Ladrillo 18 huecos limpio</t>
+  </si>
+  <si>
+    <t>Ladrillo 18 huecos semi limpio</t>
+  </si>
+  <si>
+    <t>Ladrillo techo 12x30</t>
+  </si>
+  <si>
+    <t>Ladrillo techo 15x30</t>
+  </si>
+  <si>
+    <t>Ladrillo techo 8x30</t>
+  </si>
+  <si>
+    <t>Llave termica 16 - bticino</t>
+  </si>
+  <si>
+    <t>Llave termica 20 - bticino</t>
+  </si>
+  <si>
+    <t>Llave termica 32 - bticino</t>
+  </si>
+  <si>
+    <t>Llave termica 60 - bticino</t>
+  </si>
+  <si>
+    <t>Llave termica 60 - stronger</t>
+  </si>
+  <si>
+    <t>Niple 1/2"</t>
+  </si>
+  <si>
+    <t>Niple bronce 1/2"</t>
+  </si>
+  <si>
+    <t>Pegamento PVC 1/16" azul</t>
+  </si>
+  <si>
+    <t>Pegamento PVC 1/16" dorado</t>
+  </si>
+  <si>
+    <t>Pegamento PVC 1/32" azul</t>
+  </si>
+  <si>
+    <t>Pegamento PVC 1/32" dorado</t>
+  </si>
+  <si>
+    <t>Pegamento PVC 1/4" dorado</t>
+  </si>
+  <si>
+    <t>Pegamento PVC 1/8" azul</t>
+  </si>
+  <si>
+    <t>Pegamento PVC 1/8" dorado</t>
+  </si>
+  <si>
+    <t>Pegamento PVC agua caliente</t>
+  </si>
+  <si>
+    <t>Pegamento polvo - celima</t>
+  </si>
+  <si>
+    <t>Reduccion desague 4"a2"</t>
+  </si>
+  <si>
+    <t>Rodillo 12" - toro</t>
+  </si>
+  <si>
+    <t>Rodillo 9" - toro</t>
+  </si>
+  <si>
+    <t>Tee bronce 1/2"</t>
+  </si>
+  <si>
+    <t>Tee agua 1/2"</t>
+  </si>
+  <si>
+    <t>Tee agua 3/4"</t>
+  </si>
+  <si>
+    <t>Tee agua caliente 1/2"</t>
+  </si>
+  <si>
+    <t>Tee desague 4" x 2"</t>
+  </si>
+  <si>
+    <t>Tee desague 4" x 4"</t>
+  </si>
+  <si>
+    <t>Tee desague sanitaria 2"</t>
+  </si>
+  <si>
+    <t>Tubo agua 1/2"</t>
+  </si>
+  <si>
+    <t>Tubo agua 3/4"</t>
+  </si>
+  <si>
+    <t>Tubo agua caliente 1/2"</t>
+  </si>
+  <si>
+    <t>Tubo desague 2"</t>
+  </si>
+  <si>
+    <t>Tubo desague 3"</t>
+  </si>
+  <si>
+    <t>Tubo desague 4"</t>
+  </si>
+  <si>
+    <t>Tubo luz 1"</t>
+  </si>
+  <si>
+    <t>Tubo luz 3/4"</t>
+  </si>
+  <si>
+    <t>Union bronce 1/2"</t>
+  </si>
+  <si>
+    <t>Union agua 1/2"</t>
+  </si>
+  <si>
+    <t>Union agua 3/4"</t>
+  </si>
+  <si>
+    <t>Visagra 3" (par)</t>
+  </si>
+  <si>
+    <t>Visagra 3" - capuchino (par)</t>
+  </si>
+  <si>
+    <t>Yee desague 2"</t>
+  </si>
+  <si>
+    <t>Yee sanitario 2"</t>
+  </si>
+  <si>
+    <t>Yee sanitario 4"</t>
+  </si>
+  <si>
+    <t>Yee desague 4"x2"</t>
+  </si>
+  <si>
+    <t>Yee desague 4"x4"</t>
+  </si>
+  <si>
+    <t>Yee sanitario 4"x2"</t>
+  </si>
+  <si>
+    <t>Parante 3m</t>
+  </si>
+  <si>
+    <t>Parante 2.5m</t>
+  </si>
+  <si>
+    <t>Liston 3m</t>
+  </si>
+  <si>
+    <t>Liston 2.5m</t>
+  </si>
+  <si>
+    <t>Clavo 2"y1/2"</t>
   </si>
 </sst>
 </file>
@@ -3121,10 +3424,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N129"/>
+  <dimension ref="A1:N130"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3205,7 +3508,7 @@
         <v>241</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>159</v>
+        <v>281</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
@@ -3215,7 +3518,7 @@
       </c>
       <c r="H3" t="str">
         <f t="shared" ref="H3:H66" si="0">C3</f>
-        <v>Adaptador de agua 1/2"</v>
+        <v>Adaptador agua 1/2"</v>
       </c>
       <c r="I3" s="7" t="s">
         <v>266</v>
@@ -3236,7 +3539,7 @@
       </c>
       <c r="N3" t="str">
         <f t="shared" ref="N3:N66" si="3">CONCATENATE(G3,H3,I3,J3,K3,L3,M3)</f>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Adaptador de agua 1/2"', 1, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Adaptador agua 1/2"', 1, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -3248,7 +3551,7 @@
         <v>241</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>160</v>
+        <v>282</v>
       </c>
       <c r="D4" s="3">
         <v>2.5</v>
@@ -3258,7 +3561,7 @@
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
-        <v>Adaptador de agua 3/4"</v>
+        <v>Adaptador agua 3/4"</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>266</v>
@@ -3279,7 +3582,7 @@
       </c>
       <c r="N4" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Adaptador de agua 3/4"', 2.5, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Adaptador agua 3/4"', 2.5, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -3291,7 +3594,7 @@
         <v>241</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>162</v>
+        <v>283</v>
       </c>
       <c r="D5" s="3">
         <v>1</v>
@@ -3301,7 +3604,7 @@
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
-        <v>Adaptador de agua caliente 1/2"</v>
+        <v>Adaptador agua 1/2" caliente</v>
       </c>
       <c r="I5" s="7" t="s">
         <v>266</v>
@@ -3322,7 +3625,7 @@
       </c>
       <c r="N5" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Adaptador de agua caliente 1/2"', 1, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Adaptador agua 1/2" caliente', 1, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -3334,7 +3637,7 @@
         <v>242</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>195</v>
+        <v>284</v>
       </c>
       <c r="D6" s="3">
         <v>4</v>
@@ -3344,7 +3647,7 @@
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
-        <v>Alambre N° 16</v>
+        <v>Alambre N16</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>266</v>
@@ -3365,7 +3668,7 @@
       </c>
       <c r="N6" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Alambre N° 16', 4, 'Activo', 0, 0, 6 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Alambre N16', 4, 'Activo', 0, 0, 6 ) ; </v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -3377,7 +3680,7 @@
         <v>242</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>194</v>
+        <v>285</v>
       </c>
       <c r="D7" s="3">
         <v>4</v>
@@ -3387,7 +3690,7 @@
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
-        <v>Alambre N° 8</v>
+        <v>Alambre N8</v>
       </c>
       <c r="I7" s="7" t="s">
         <v>266</v>
@@ -3408,7 +3711,7 @@
       </c>
       <c r="N7" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Alambre N° 8', 4, 'Activo', 0, 0, 6 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Alambre N8', 4, 'Activo', 0, 0, 6 ) ; </v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -3506,7 +3809,7 @@
         <v>243</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>197</v>
+        <v>286</v>
       </c>
       <c r="D10" s="3">
         <v>145</v>
@@ -3516,7 +3819,7 @@
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
-        <v>Cable de luz N° 12</v>
+        <v>Cable de luz N12</v>
       </c>
       <c r="I10" s="7" t="s">
         <v>266</v>
@@ -3537,7 +3840,7 @@
       </c>
       <c r="N10" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Cable de luz N° 12', 145, 'Activo', 0, 0, 10 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Cable de luz N12', 145, 'Activo', 0, 0, 10 ) ; </v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -3549,7 +3852,7 @@
         <v>243</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>196</v>
+        <v>287</v>
       </c>
       <c r="D11" s="3">
         <v>80</v>
@@ -3559,7 +3862,7 @@
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
-        <v>Cable de luz N° 14</v>
+        <v>Cable de luz N14</v>
       </c>
       <c r="I11" s="7" t="s">
         <v>266</v>
@@ -3580,7 +3883,7 @@
       </c>
       <c r="N11" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Cable de luz N° 14', 80, 'Activo', 0, 0, 10 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Cable de luz N14', 80, 'Activo', 0, 0, 10 ) ; </v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -3592,24 +3895,24 @@
         <v>241</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>207</v>
+        <v>288</v>
       </c>
       <c r="D12" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G12" t="s">
         <v>267</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
-        <v>Calamina de 3.0 m</v>
+        <v>Calamina 3.0m</v>
       </c>
       <c r="I12" s="7" t="s">
         <v>266</v>
       </c>
       <c r="J12" s="3">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K12" t="s">
         <v>269</v>
@@ -3623,7 +3926,7 @@
       </c>
       <c r="N12" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Calamina de 3.0 m', 12, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Calamina 3.0m', 13, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -3635,24 +3938,24 @@
         <v>241</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>206</v>
+        <v>289</v>
       </c>
       <c r="D13" s="3">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G13" t="s">
         <v>267</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
-        <v>Calamina de 3.6 m</v>
+        <v>Calamina 3.6m</v>
       </c>
       <c r="I13" s="7" t="s">
         <v>266</v>
       </c>
       <c r="J13" s="3">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K13" t="s">
         <v>269</v>
@@ -3666,7 +3969,7 @@
       </c>
       <c r="N13" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Calamina de 3.6 m', 14, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Calamina 3.6m', 15, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -3936,7 +4239,7 @@
         <v>242</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>182</v>
+        <v>290</v>
       </c>
       <c r="D20" s="3">
         <v>8</v>
@@ -3946,7 +4249,7 @@
       </c>
       <c r="H20" t="str">
         <f t="shared" si="0"/>
-        <v>Clavo de 1 y 1/2"</v>
+        <v>Clavo 1y1/2"</v>
       </c>
       <c r="I20" s="7" t="s">
         <v>266</v>
@@ -3967,7 +4270,7 @@
       </c>
       <c r="N20" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Clavo de 1 y 1/2"', 8, 'Activo', 0, 0, 6 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Clavo 1y1/2"', 8, 'Activo', 0, 0, 6 ) ; </v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -3979,7 +4282,7 @@
         <v>242</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>181</v>
+        <v>291</v>
       </c>
       <c r="D21" s="3">
         <v>8</v>
@@ -3989,7 +4292,7 @@
       </c>
       <c r="H21" t="str">
         <f t="shared" si="0"/>
-        <v>Clavo de 1"</v>
+        <v>Clavo 1"</v>
       </c>
       <c r="I21" s="7" t="s">
         <v>266</v>
@@ -4010,7 +4313,7 @@
       </c>
       <c r="N21" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Clavo de 1"', 8, 'Activo', 0, 0, 6 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Clavo 1"', 8, 'Activo', 0, 0, 6 ) ; </v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -4022,7 +4325,7 @@
         <v>242</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>180</v>
+        <v>292</v>
       </c>
       <c r="D22" s="3">
         <v>4.5</v>
@@ -4032,7 +4335,7 @@
       </c>
       <c r="H22" t="str">
         <f t="shared" si="0"/>
-        <v>Clavo de 2"</v>
+        <v>Clavo 2"</v>
       </c>
       <c r="I22" s="7" t="s">
         <v>266</v>
@@ -4053,7 +4356,7 @@
       </c>
       <c r="N22" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Clavo de 2"', 4.5, 'Activo', 0, 0, 6 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Clavo 2"', 4.5, 'Activo', 0, 0, 6 ) ; </v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -4065,7 +4368,7 @@
         <v>242</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>179</v>
+        <v>293</v>
       </c>
       <c r="D23" s="3">
         <v>4.5</v>
@@ -4075,7 +4378,7 @@
       </c>
       <c r="H23" t="str">
         <f t="shared" si="0"/>
-        <v>Clavo de 3"</v>
+        <v>Clavo 3"</v>
       </c>
       <c r="I23" s="7" t="s">
         <v>266</v>
@@ -4096,7 +4399,7 @@
       </c>
       <c r="N23" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Clavo de 3"', 4.5, 'Activo', 0, 0, 6 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Clavo 3"', 4.5, 'Activo', 0, 0, 6 ) ; </v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -4108,7 +4411,7 @@
         <v>242</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>178</v>
+        <v>294</v>
       </c>
       <c r="D24" s="3">
         <v>4.5</v>
@@ -4118,7 +4421,7 @@
       </c>
       <c r="H24" t="str">
         <f t="shared" si="0"/>
-        <v>Clavo de 4"</v>
+        <v>Clavo 4"</v>
       </c>
       <c r="I24" s="7" t="s">
         <v>266</v>
@@ -4139,7 +4442,7 @@
       </c>
       <c r="N24" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Clavo de 4"', 4.5, 'Activo', 0, 0, 6 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Clavo 4"', 4.5, 'Activo', 0, 0, 6 ) ; </v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -4151,7 +4454,7 @@
         <v>245</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>184</v>
+        <v>295</v>
       </c>
       <c r="D25" s="3">
         <v>9</v>
@@ -4161,7 +4464,7 @@
       </c>
       <c r="H25" t="str">
         <f t="shared" si="0"/>
-        <v>Clavo de acero 2"</v>
+        <v>Clavo acero 2"</v>
       </c>
       <c r="I25" s="7" t="s">
         <v>266</v>
@@ -4182,7 +4485,7 @@
       </c>
       <c r="N25" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Clavo de acero 2"', 9, 'Activo', 0, 0, 11 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Clavo acero 2"', 9, 'Activo', 0, 0, 11 ) ; </v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -4194,7 +4497,7 @@
         <v>245</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>185</v>
+        <v>296</v>
       </c>
       <c r="D26" s="3">
         <v>9</v>
@@ -4204,7 +4507,7 @@
       </c>
       <c r="H26" t="str">
         <f t="shared" si="0"/>
-        <v>Clavo de acero 3"</v>
+        <v>Clavo acero 3"</v>
       </c>
       <c r="I26" s="7" t="s">
         <v>266</v>
@@ -4225,7 +4528,7 @@
       </c>
       <c r="N26" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Clavo de acero 3"', 9, 'Activo', 0, 0, 11 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Clavo acero 3"', 9, 'Activo', 0, 0, 11 ) ; </v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -4237,7 +4540,7 @@
         <v>245</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>186</v>
+        <v>297</v>
       </c>
       <c r="D27" s="3">
         <v>9</v>
@@ -4247,7 +4550,7 @@
       </c>
       <c r="H27" t="str">
         <f t="shared" si="0"/>
-        <v>Clavo de acero 4"</v>
+        <v>Clavo acero 4"</v>
       </c>
       <c r="I27" s="7" t="s">
         <v>266</v>
@@ -4268,7 +4571,7 @@
       </c>
       <c r="N27" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Clavo de acero 4"', 9, 'Activo', 0, 0, 11 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Clavo acero 4"', 9, 'Activo', 0, 0, 11 ) ; </v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -4280,7 +4583,7 @@
         <v>242</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>183</v>
+        <v>298</v>
       </c>
       <c r="D28" s="3">
         <v>8</v>
@@ -4290,7 +4593,7 @@
       </c>
       <c r="H28" t="str">
         <f t="shared" si="0"/>
-        <v>Clavo de calamina</v>
+        <v>Clavo calamina</v>
       </c>
       <c r="I28" s="7" t="s">
         <v>266</v>
@@ -4311,7 +4614,7 @@
       </c>
       <c r="N28" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Clavo de calamina', 8, 'Activo', 0, 0, 6 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Clavo calamina', 8, 'Activo', 0, 0, 6 ) ; </v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -4323,7 +4626,7 @@
         <v>241</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>280</v>
+        <v>299</v>
       </c>
       <c r="D29" s="3">
         <v>4.5</v>
@@ -4333,7 +4636,7 @@
       </c>
       <c r="H29" t="str">
         <f t="shared" si="0"/>
-        <v>Codo bronce de 1/2"</v>
+        <v>Codo bronce 1/2"</v>
       </c>
       <c r="I29" s="7" t="s">
         <v>266</v>
@@ -4354,7 +4657,7 @@
       </c>
       <c r="N29" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Codo bronce de 1/2"', 4.5, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Codo bronce 1/2"', 4.5, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -4366,7 +4669,7 @@
         <v>241</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>143</v>
+        <v>300</v>
       </c>
       <c r="D30" s="3">
         <v>1</v>
@@ -4376,7 +4679,7 @@
       </c>
       <c r="H30" t="str">
         <f t="shared" si="0"/>
-        <v>Codo de agua 1/2"</v>
+        <v>Codo agua 1/2"</v>
       </c>
       <c r="I30" s="7" t="s">
         <v>266</v>
@@ -4397,7 +4700,7 @@
       </c>
       <c r="N30" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Codo de agua 1/2"', 1, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Codo agua 1/2"', 1, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
@@ -4409,7 +4712,7 @@
         <v>241</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>139</v>
+        <v>301</v>
       </c>
       <c r="D31" s="3">
         <v>2.5</v>
@@ -4419,7 +4722,7 @@
       </c>
       <c r="H31" t="str">
         <f t="shared" si="0"/>
-        <v>Codo de agua 3/4" 45°</v>
+        <v>Codo agua 3/4" 45°</v>
       </c>
       <c r="I31" s="7" t="s">
         <v>266</v>
@@ -4440,7 +4743,7 @@
       </c>
       <c r="N31" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Codo de agua 3/4" 45°', 2.5, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Codo agua 3/4" 45°', 2.5, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
@@ -4452,7 +4755,7 @@
         <v>241</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>142</v>
+        <v>302</v>
       </c>
       <c r="D32" s="3">
         <v>2.5</v>
@@ -4462,7 +4765,7 @@
       </c>
       <c r="H32" t="str">
         <f t="shared" si="0"/>
-        <v>Codo de agua 3/4" 90°</v>
+        <v>Codo agua 3/4" 90°</v>
       </c>
       <c r="I32" s="7" t="s">
         <v>266</v>
@@ -4483,7 +4786,7 @@
       </c>
       <c r="N32" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Codo de agua 3/4" 90°', 2.5, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Codo agua 3/4" 90°', 2.5, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
@@ -4495,7 +4798,7 @@
         <v>241</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>161</v>
+        <v>306</v>
       </c>
       <c r="D33" s="3">
         <v>1</v>
@@ -4505,7 +4808,7 @@
       </c>
       <c r="H33" t="str">
         <f t="shared" si="0"/>
-        <v>Codo de agua caliente 1/2"</v>
+        <v>Codo agua caliente 1/2"</v>
       </c>
       <c r="I33" s="7" t="s">
         <v>266</v>
@@ -4526,7 +4829,7 @@
       </c>
       <c r="N33" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Codo de agua caliente 1/2"', 1, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Codo agua caliente 1/2"', 1, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
@@ -4538,7 +4841,7 @@
         <v>241</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>141</v>
+        <v>303</v>
       </c>
       <c r="D34" s="3">
         <v>1.5</v>
@@ -4548,7 +4851,7 @@
       </c>
       <c r="H34" t="str">
         <f t="shared" si="0"/>
-        <v>Codo de desague 2" 45°</v>
+        <v>Codo desague 2" 45°</v>
       </c>
       <c r="I34" s="7" t="s">
         <v>266</v>
@@ -4569,7 +4872,7 @@
       </c>
       <c r="N34" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Codo de desague 2" 45°', 1.5, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Codo desague 2" 45°', 1.5, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
@@ -4581,7 +4884,7 @@
         <v>241</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>140</v>
+        <v>304</v>
       </c>
       <c r="D35" s="3">
         <v>1.5</v>
@@ -4591,7 +4894,7 @@
       </c>
       <c r="H35" t="str">
         <f t="shared" si="0"/>
-        <v>Codo de desague 2" 90°</v>
+        <v>Codo desague 2" 90°</v>
       </c>
       <c r="I35" s="7" t="s">
         <v>266</v>
@@ -4612,7 +4915,7 @@
       </c>
       <c r="N35" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Codo de desague 2" 90°', 1.5, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Codo desague 2" 90°', 1.5, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
@@ -4624,7 +4927,7 @@
         <v>241</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>138</v>
+        <v>305</v>
       </c>
       <c r="D36" s="3">
         <v>5</v>
@@ -4634,7 +4937,7 @@
       </c>
       <c r="H36" t="str">
         <f t="shared" si="0"/>
-        <v>Codo de desague 4" 45°</v>
+        <v>Codo desague 4" 45°</v>
       </c>
       <c r="I36" s="7" t="s">
         <v>266</v>
@@ -4655,7 +4958,7 @@
       </c>
       <c r="N36" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Codo de desague 4" 45°', 5, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Codo desague 4" 45°', 5, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
@@ -4667,7 +4970,7 @@
         <v>241</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>137</v>
+        <v>307</v>
       </c>
       <c r="D37" s="3">
         <v>5</v>
@@ -4677,7 +4980,7 @@
       </c>
       <c r="H37" t="str">
         <f t="shared" si="0"/>
-        <v>Codo de desague 4" 90°</v>
+        <v>Codo desague 4" 90°</v>
       </c>
       <c r="I37" s="7" t="s">
         <v>266</v>
@@ -4698,7 +5001,7 @@
       </c>
       <c r="N37" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Codo de desague 4" 90°', 5, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Codo desague 4" 90°', 5, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
@@ -4710,7 +5013,7 @@
         <v>241</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>144</v>
+        <v>308</v>
       </c>
       <c r="D38" s="3">
         <v>7</v>
@@ -4720,7 +5023,7 @@
       </c>
       <c r="H38" t="str">
         <f t="shared" si="0"/>
-        <v>Codo de desague 4" a 2"</v>
+        <v>Codo desague 4"a2"</v>
       </c>
       <c r="I38" s="7" t="s">
         <v>266</v>
@@ -4741,7 +5044,7 @@
       </c>
       <c r="N38" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Codo de desague 4" a 2"', 7, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Codo desague 4"a2"', 7, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
@@ -4753,7 +5056,7 @@
         <v>241</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>145</v>
+        <v>309</v>
       </c>
       <c r="D39" s="3">
         <v>1</v>
@@ -4763,7 +5066,7 @@
       </c>
       <c r="H39" t="str">
         <f t="shared" si="0"/>
-        <v>Codo de luz 1"</v>
+        <v>Codo luz 1"</v>
       </c>
       <c r="I39" s="7" t="s">
         <v>266</v>
@@ -4784,7 +5087,7 @@
       </c>
       <c r="N39" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Codo de luz 1"', 1, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Codo luz 1"', 1, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
@@ -4796,7 +5099,7 @@
         <v>241</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>146</v>
+        <v>310</v>
       </c>
       <c r="D40" s="3">
         <v>0.5</v>
@@ -4806,7 +5109,7 @@
       </c>
       <c r="H40" t="str">
         <f t="shared" si="0"/>
-        <v>Codo de luz 3/4"</v>
+        <v>Codo luz 3/4"</v>
       </c>
       <c r="I40" s="7" t="s">
         <v>266</v>
@@ -4827,7 +5130,7 @@
       </c>
       <c r="N40" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Codo de luz 3/4"', 0.5, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Codo luz 3/4"', 0.5, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
@@ -4839,7 +5142,7 @@
         <v>241</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>165</v>
+        <v>311</v>
       </c>
       <c r="D41" s="3">
         <v>1.5</v>
@@ -4849,7 +5152,7 @@
       </c>
       <c r="H41" t="str">
         <f t="shared" si="0"/>
-        <v>Codo galvanizado de 1/2"</v>
+        <v>Codo galvanizado 1/2"</v>
       </c>
       <c r="I41" s="7" t="s">
         <v>266</v>
@@ -4870,7 +5173,7 @@
       </c>
       <c r="N41" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Codo galvanizado de 1/2"', 1.5, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Codo galvanizado 1/2"', 1.5, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
@@ -4882,7 +5185,7 @@
         <v>241</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>235</v>
+        <v>312</v>
       </c>
       <c r="D42" s="3">
         <v>20</v>
@@ -4892,7 +5195,7 @@
       </c>
       <c r="H42" t="str">
         <f t="shared" si="0"/>
-        <v>Disco corte fierro de 14"</v>
+        <v>Disco corte fierro 14"</v>
       </c>
       <c r="I42" s="7" t="s">
         <v>266</v>
@@ -4913,7 +5216,7 @@
       </c>
       <c r="N42" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Disco corte fierro de 14"', 20, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Disco corte fierro 14"', 20, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
@@ -4925,7 +5228,7 @@
         <v>241</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>232</v>
+        <v>313</v>
       </c>
       <c r="D43" s="3">
         <v>5</v>
@@ -4935,7 +5238,7 @@
       </c>
       <c r="H43" t="str">
         <f t="shared" si="0"/>
-        <v>Disco corte fierro de 4"</v>
+        <v>Disco corte fierro 4"</v>
       </c>
       <c r="I43" s="7" t="s">
         <v>266</v>
@@ -4956,7 +5259,7 @@
       </c>
       <c r="N43" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Disco corte fierro de 4"', 5, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Disco corte fierro 4"', 5, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
@@ -4968,7 +5271,7 @@
         <v>241</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>233</v>
+        <v>314</v>
       </c>
       <c r="D44" s="3">
         <v>8</v>
@@ -4978,7 +5281,7 @@
       </c>
       <c r="H44" t="str">
         <f t="shared" si="0"/>
-        <v>Disco corte fierro de 7"</v>
+        <v>Disco corte fierro 7"</v>
       </c>
       <c r="I44" s="7" t="s">
         <v>266</v>
@@ -4999,7 +5302,7 @@
       </c>
       <c r="N44" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Disco corte fierro de 7"', 8, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Disco corte fierro 7"', 8, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
@@ -5011,7 +5314,7 @@
         <v>241</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>234</v>
+        <v>315</v>
       </c>
       <c r="D45" s="3">
         <v>12</v>
@@ -5021,7 +5324,7 @@
       </c>
       <c r="H45" t="str">
         <f t="shared" si="0"/>
-        <v>Disco corte fierro de 9"</v>
+        <v>Disco corte fierro 9"</v>
       </c>
       <c r="I45" s="7" t="s">
         <v>266</v>
@@ -5042,7 +5345,7 @@
       </c>
       <c r="N45" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Disco corte fierro de 9"', 12, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Disco corte fierro 9"', 12, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
@@ -5054,7 +5357,7 @@
         <v>241</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>237</v>
+        <v>316</v>
       </c>
       <c r="D46" s="3">
         <v>15</v>
@@ -5064,7 +5367,7 @@
       </c>
       <c r="H46" t="str">
         <f t="shared" si="0"/>
-        <v>Disco para concreto de 15" - dinamo</v>
+        <v>Disco para concreto 15" - dinamo</v>
       </c>
       <c r="I46" s="7" t="s">
         <v>266</v>
@@ -5085,7 +5388,7 @@
       </c>
       <c r="N46" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Disco para concreto de 15" - dinamo', 15, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Disco para concreto 15" - dinamo', 15, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
@@ -5097,7 +5400,7 @@
         <v>241</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>240</v>
+        <v>317</v>
       </c>
       <c r="D47" s="3">
         <v>22</v>
@@ -5107,7 +5410,7 @@
       </c>
       <c r="H47" t="str">
         <f t="shared" si="0"/>
-        <v>Disco para concreto de 15" - kamasa</v>
+        <v>Disco para concreto 15" - kamasa</v>
       </c>
       <c r="I47" s="7" t="s">
         <v>266</v>
@@ -5128,7 +5431,7 @@
       </c>
       <c r="N47" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Disco para concreto de 15" - kamasa', 22, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Disco para concreto 15" - kamasa', 22, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
@@ -5140,7 +5443,7 @@
         <v>241</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>238</v>
+        <v>318</v>
       </c>
       <c r="D48" s="3">
         <v>30</v>
@@ -5150,7 +5453,7 @@
       </c>
       <c r="H48" t="str">
         <f t="shared" si="0"/>
-        <v>Disco para concreto de 30" - dinamo</v>
+        <v>Disco para concreto 30" - dinamo</v>
       </c>
       <c r="I48" s="7" t="s">
         <v>266</v>
@@ -5171,7 +5474,7 @@
       </c>
       <c r="N48" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Disco para concreto de 30" - dinamo', 30, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Disco para concreto 30" - dinamo', 30, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
@@ -5183,7 +5486,7 @@
         <v>241</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>236</v>
+        <v>319</v>
       </c>
       <c r="D49" s="3">
         <v>8</v>
@@ -5193,7 +5496,7 @@
       </c>
       <c r="H49" t="str">
         <f t="shared" si="0"/>
-        <v>Disco para concreto de 4" - dinamo</v>
+        <v>Disco para concreto 4" - dinamo</v>
       </c>
       <c r="I49" s="7" t="s">
         <v>266</v>
@@ -5214,7 +5517,7 @@
       </c>
       <c r="N49" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Disco para concreto de 4" - dinamo', 8, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Disco para concreto 4" - dinamo', 8, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
@@ -5226,7 +5529,7 @@
         <v>241</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>239</v>
+        <v>320</v>
       </c>
       <c r="D50" s="3">
         <v>9</v>
@@ -5236,7 +5539,7 @@
       </c>
       <c r="H50" t="str">
         <f t="shared" si="0"/>
-        <v>Disco para concreto de 4" - kamasa</v>
+        <v>Disco para concreto 4" - kamasa</v>
       </c>
       <c r="I50" s="7" t="s">
         <v>266</v>
@@ -5257,7 +5560,7 @@
       </c>
       <c r="N50" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Disco para concreto de 4" - kamasa', 9, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Disco para concreto 4" - kamasa', 9, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
@@ -5398,7 +5701,7 @@
         <v>246</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>222</v>
+        <v>321</v>
       </c>
       <c r="D54" s="3">
         <v>25.5</v>
@@ -5408,7 +5711,7 @@
       </c>
       <c r="H54" t="str">
         <f t="shared" si="0"/>
-        <v>Fierro de 1/2" - siderperu</v>
+        <v>Fierro 1/2" - siderperu</v>
       </c>
       <c r="I54" s="7" t="s">
         <v>266</v>
@@ -5429,7 +5732,7 @@
       </c>
       <c r="N54" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Fierro de 1/2" - siderperu', 25.5, 'Activo', 0, 0, 4 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Fierro 1/2" - siderperu', 25.5, 'Activo', 0, 0, 4 ) ; </v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
@@ -5441,7 +5744,7 @@
         <v>246</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>225</v>
+        <v>322</v>
       </c>
       <c r="D55" s="3">
         <v>6.5</v>
@@ -5451,7 +5754,7 @@
       </c>
       <c r="H55" t="str">
         <f t="shared" si="0"/>
-        <v>Fierro de 1/4" 6mm - siderperu</v>
+        <v>Fierro 1/4" 6mm - siderperu</v>
       </c>
       <c r="I55" s="7" t="s">
         <v>266</v>
@@ -5472,7 +5775,7 @@
       </c>
       <c r="N55" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Fierro de 1/4" 6mm - siderperu', 6.5, 'Activo', 0, 0, 4 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Fierro 1/4" 6mm - siderperu', 6.5, 'Activo', 0, 0, 4 ) ; </v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
@@ -5484,7 +5787,7 @@
         <v>246</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>220</v>
+        <v>323</v>
       </c>
       <c r="D56" s="3">
         <v>58</v>
@@ -5494,7 +5797,7 @@
       </c>
       <c r="H56" t="str">
         <f t="shared" si="0"/>
-        <v>Fierro de 3/4" - siderperu</v>
+        <v>Fierro 3/4" - siderperu</v>
       </c>
       <c r="I56" s="7" t="s">
         <v>266</v>
@@ -5515,7 +5818,7 @@
       </c>
       <c r="N56" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Fierro de 3/4" - siderperu', 58, 'Activo', 0, 0, 4 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Fierro 3/4" - siderperu', 58, 'Activo', 0, 0, 4 ) ; </v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
@@ -5527,7 +5830,7 @@
         <v>246</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>223</v>
+        <v>324</v>
       </c>
       <c r="D57" s="3">
         <v>15</v>
@@ -5537,7 +5840,7 @@
       </c>
       <c r="H57" t="str">
         <f t="shared" si="0"/>
-        <v>Fierro de 3/8" - siderperu</v>
+        <v>Fierro 3/8" - siderperu</v>
       </c>
       <c r="I57" s="7" t="s">
         <v>266</v>
@@ -5558,7 +5861,7 @@
       </c>
       <c r="N57" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Fierro de 3/8" - siderperu', 15, 'Activo', 0, 0, 4 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Fierro 3/8" - siderperu', 15, 'Activo', 0, 0, 4 ) ; </v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
@@ -5570,7 +5873,7 @@
         <v>246</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>276</v>
+        <v>325</v>
       </c>
       <c r="D58" s="3">
         <v>39.5</v>
@@ -5580,7 +5883,7 @@
       </c>
       <c r="H58" t="str">
         <f t="shared" si="0"/>
-        <v>Fierro de 5/8" - siderperu</v>
+        <v>Fierro 5/8" - siderperu</v>
       </c>
       <c r="I58" s="7" t="s">
         <v>266</v>
@@ -5601,7 +5904,7 @@
       </c>
       <c r="N58" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Fierro de 5/8" - siderperu', 39.5, 'Activo', 0, 0, 4 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Fierro 5/8" - siderperu', 39.5, 'Activo', 0, 0, 4 ) ; </v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
@@ -5613,7 +5916,7 @@
         <v>246</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>224</v>
+        <v>326</v>
       </c>
       <c r="D59" s="3">
         <v>11</v>
@@ -5623,7 +5926,7 @@
       </c>
       <c r="H59" t="str">
         <f t="shared" si="0"/>
-        <v>Fierro de 8mm - siderperu</v>
+        <v>Fierro 8mm - siderperu</v>
       </c>
       <c r="I59" s="7" t="s">
         <v>266</v>
@@ -5644,7 +5947,7 @@
       </c>
       <c r="N59" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Fierro de 8mm - siderperu', 11, 'Activo', 0, 0, 4 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Fierro 8mm - siderperu', 11, 'Activo', 0, 0, 4 ) ; </v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
@@ -5656,7 +5959,7 @@
         <v>241</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>230</v>
+        <v>327</v>
       </c>
       <c r="D60" s="3">
         <v>5</v>
@@ -5666,7 +5969,7 @@
       </c>
       <c r="H60" t="str">
         <f t="shared" si="0"/>
-        <v>Foco de 27 W</v>
+        <v>Foco 27 W</v>
       </c>
       <c r="I60" s="7" t="s">
         <v>266</v>
@@ -5687,7 +5990,7 @@
       </c>
       <c r="N60" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Foco de 27 W', 5, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Foco 27 W', 5, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
@@ -5699,7 +6002,7 @@
         <v>241</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>229</v>
+        <v>328</v>
       </c>
       <c r="D61" s="3">
         <v>6.5</v>
@@ -5709,7 +6012,7 @@
       </c>
       <c r="H61" t="str">
         <f t="shared" si="0"/>
-        <v>Foco de 32 W</v>
+        <v>Foco 32 W</v>
       </c>
       <c r="I61" s="7" t="s">
         <v>266</v>
@@ -5730,7 +6033,7 @@
       </c>
       <c r="N61" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Foco de 32 W', 6.5, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Foco 32 W', 6.5, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
@@ -5742,7 +6045,7 @@
         <v>241</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>228</v>
+        <v>329</v>
       </c>
       <c r="D62" s="3">
         <v>7</v>
@@ -5752,7 +6055,7 @@
       </c>
       <c r="H62" t="str">
         <f t="shared" si="0"/>
-        <v>Foco de 42 W</v>
+        <v>Foco 42 W</v>
       </c>
       <c r="I62" s="7" t="s">
         <v>266</v>
@@ -5773,7 +6076,7 @@
       </c>
       <c r="N62" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Foco de 42 W', 7, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Foco 42 W', 7, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
@@ -5785,7 +6088,7 @@
         <v>241</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>227</v>
+        <v>330</v>
       </c>
       <c r="D63" s="3">
         <v>14</v>
@@ -5795,7 +6098,7 @@
       </c>
       <c r="H63" t="str">
         <f t="shared" si="0"/>
-        <v>Foco de 85 W</v>
+        <v>Foco 85 W</v>
       </c>
       <c r="I63" s="7" t="s">
         <v>266</v>
@@ -5816,7 +6119,7 @@
       </c>
       <c r="N63" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Foco de 85 W', 14, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Foco 85 W', 14, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
@@ -5828,7 +6131,7 @@
         <v>241</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>231</v>
+        <v>331</v>
       </c>
       <c r="D64" s="3">
         <v>13</v>
@@ -5838,7 +6141,7 @@
       </c>
       <c r="H64" t="str">
         <f t="shared" si="0"/>
-        <v>Foco LED de 7 W</v>
+        <v>Foco LED 7 W</v>
       </c>
       <c r="I64" s="7" t="s">
         <v>266</v>
@@ -5859,7 +6162,7 @@
       </c>
       <c r="N64" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Foco LED de 7 W', 13, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Foco LED 7 W', 13, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.25">
@@ -5871,7 +6174,7 @@
         <v>247</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>202</v>
+        <v>332</v>
       </c>
       <c r="D65" s="3">
         <v>670</v>
@@ -5881,7 +6184,7 @@
       </c>
       <c r="H65" t="str">
         <f t="shared" si="0"/>
-        <v>Ladrillo de 18 huecos limpio (millar)</v>
+        <v>Ladrillo 18 huecos limpio</v>
       </c>
       <c r="I65" s="7" t="s">
         <v>266</v>
@@ -5902,7 +6205,7 @@
       </c>
       <c r="N65" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Ladrillo de 18 huecos limpio (millar)', 670, 'Activo', 0, 0, 12 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Ladrillo 18 huecos limpio', 670, 'Activo', 0, 0, 12 ) ; </v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.25">
@@ -5914,7 +6217,7 @@
         <v>247</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>203</v>
+        <v>333</v>
       </c>
       <c r="D66" s="3">
         <v>560</v>
@@ -5924,7 +6227,7 @@
       </c>
       <c r="H66" t="str">
         <f t="shared" si="0"/>
-        <v>Ladrillo de 18 huecos semi limpio (millar)</v>
+        <v>Ladrillo 18 huecos semi limpio</v>
       </c>
       <c r="I66" s="7" t="s">
         <v>266</v>
@@ -5945,7 +6248,7 @@
       </c>
       <c r="N66" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Ladrillo de 18 huecos semi limpio (millar)', 560, 'Activo', 0, 0, 12 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Ladrillo 18 huecos semi limpio', 560, 'Activo', 0, 0, 12 ) ; </v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.25">
@@ -5957,7 +6260,7 @@
         <v>247</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>200</v>
+        <v>334</v>
       </c>
       <c r="D67" s="3">
         <v>2100</v>
@@ -5967,7 +6270,7 @@
       </c>
       <c r="H67" t="str">
         <f t="shared" ref="H67:H121" si="4">C67</f>
-        <v>Ladrillo de techo 12 x 30 (millar)</v>
+        <v>Ladrillo techo 12x30</v>
       </c>
       <c r="I67" s="7" t="s">
         <v>266</v>
@@ -5988,7 +6291,7 @@
       </c>
       <c r="N67" t="str">
         <f t="shared" ref="N67:N121" si="7">CONCATENATE(G67,H67,I67,J67,K67,L67,M67)</f>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Ladrillo de techo 12 x 30 (millar)', 2100, 'Activo', 0, 0, 12 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Ladrillo techo 12x30', 2100, 'Activo', 0, 0, 12 ) ; </v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.25">
@@ -6000,7 +6303,7 @@
         <v>247</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>199</v>
+        <v>335</v>
       </c>
       <c r="D68" s="3">
         <v>2100</v>
@@ -6010,7 +6313,7 @@
       </c>
       <c r="H68" t="str">
         <f t="shared" si="4"/>
-        <v>Ladrillo de techo 15 x 30 (millar)</v>
+        <v>Ladrillo techo 15x30</v>
       </c>
       <c r="I68" s="7" t="s">
         <v>266</v>
@@ -6031,7 +6334,7 @@
       </c>
       <c r="N68" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Ladrillo de techo 15 x 30 (millar)', 2100, 'Activo', 0, 0, 12 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Ladrillo techo 15x30', 2100, 'Activo', 0, 0, 12 ) ; </v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.25">
@@ -6043,7 +6346,7 @@
         <v>247</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>201</v>
+        <v>336</v>
       </c>
       <c r="D69" s="3">
         <v>2000</v>
@@ -6053,7 +6356,7 @@
       </c>
       <c r="H69" t="str">
         <f t="shared" si="4"/>
-        <v>Ladrillo de techo 8 x 30 (millar)</v>
+        <v>Ladrillo techo 8x30</v>
       </c>
       <c r="I69" s="7" t="s">
         <v>266</v>
@@ -6074,7 +6377,7 @@
       </c>
       <c r="N69" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Ladrillo de techo 8 x 30 (millar)', 2000, 'Activo', 0, 0, 12 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Ladrillo techo 8x30', 2000, 'Activo', 0, 0, 12 ) ; </v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.25">
@@ -6086,7 +6389,7 @@
         <v>247</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>204</v>
+        <v>280</v>
       </c>
       <c r="D70" s="3">
         <v>410</v>
@@ -6096,7 +6399,7 @@
       </c>
       <c r="H70" t="str">
         <f t="shared" si="4"/>
-        <v>Ladrillo pandereta (millar)</v>
+        <v>Ladrillo pandereta</v>
       </c>
       <c r="I70" s="7" t="s">
         <v>266</v>
@@ -6117,7 +6420,7 @@
       </c>
       <c r="N70" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Ladrillo pandereta (millar)', 410, 'Activo', 0, 0, 12 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Ladrillo pandereta', 410, 'Activo', 0, 0, 12 ) ; </v>
       </c>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.25">
@@ -6172,7 +6475,7 @@
         <v>241</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>189</v>
+        <v>337</v>
       </c>
       <c r="D72" s="3">
         <v>38</v>
@@ -6182,7 +6485,7 @@
       </c>
       <c r="H72" t="str">
         <f t="shared" si="4"/>
-        <v>Llave termica bticino 16</v>
+        <v>Llave termica 16 - bticino</v>
       </c>
       <c r="I72" s="7" t="s">
         <v>266</v>
@@ -6203,7 +6506,7 @@
       </c>
       <c r="N72" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Llave termica bticino 16', 38, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Llave termica 16 - bticino', 38, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.25">
@@ -6215,7 +6518,7 @@
         <v>241</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>188</v>
+        <v>338</v>
       </c>
       <c r="D73" s="3">
         <v>38</v>
@@ -6225,7 +6528,7 @@
       </c>
       <c r="H73" t="str">
         <f t="shared" si="4"/>
-        <v>Llave termica bticino 20</v>
+        <v>Llave termica 20 - bticino</v>
       </c>
       <c r="I73" s="7" t="s">
         <v>266</v>
@@ -6246,7 +6549,7 @@
       </c>
       <c r="N73" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Llave termica bticino 20', 38, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Llave termica 20 - bticino', 38, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.25">
@@ -6258,7 +6561,7 @@
         <v>241</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>187</v>
+        <v>339</v>
       </c>
       <c r="D74" s="3">
         <v>38</v>
@@ -6268,7 +6571,7 @@
       </c>
       <c r="H74" t="str">
         <f t="shared" si="4"/>
-        <v>Llave termica bticino 32</v>
+        <v>Llave termica 32 - bticino</v>
       </c>
       <c r="I74" s="7" t="s">
         <v>266</v>
@@ -6289,7 +6592,7 @@
       </c>
       <c r="N74" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Llave termica bticino 32', 38, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Llave termica 32 - bticino', 38, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.25">
@@ -6301,7 +6604,7 @@
         <v>241</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>190</v>
+        <v>340</v>
       </c>
       <c r="D75" s="3">
         <v>50</v>
@@ -6311,7 +6614,7 @@
       </c>
       <c r="H75" t="str">
         <f t="shared" si="4"/>
-        <v>Llave termica bticino 60</v>
+        <v>Llave termica 60 - bticino</v>
       </c>
       <c r="I75" s="7" t="s">
         <v>266</v>
@@ -6332,7 +6635,7 @@
       </c>
       <c r="N75" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Llave termica bticino 60', 50, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Llave termica 60 - bticino', 50, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.25">
@@ -6344,7 +6647,7 @@
         <v>241</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>191</v>
+        <v>341</v>
       </c>
       <c r="D76" s="3">
         <v>18</v>
@@ -6354,7 +6657,7 @@
       </c>
       <c r="H76" t="str">
         <f t="shared" si="4"/>
-        <v>Llave termica stronger 60</v>
+        <v>Llave termica 60 - stronger</v>
       </c>
       <c r="I76" s="7" t="s">
         <v>266</v>
@@ -6375,7 +6678,7 @@
       </c>
       <c r="N76" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Llave termica stronger 60', 18, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Llave termica 60 - stronger', 18, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.25">
@@ -6430,7 +6733,7 @@
         <v>241</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>168</v>
+        <v>343</v>
       </c>
       <c r="D78" s="3">
         <v>4</v>
@@ -6440,7 +6743,7 @@
       </c>
       <c r="H78" t="str">
         <f t="shared" si="4"/>
-        <v>Niple bronce de 1/2"</v>
+        <v>Niple bronce 1/2"</v>
       </c>
       <c r="I78" s="7" t="s">
         <v>266</v>
@@ -6461,7 +6764,7 @@
       </c>
       <c r="N78" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Niple bronce de 1/2"', 4, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Niple bronce 1/2"', 4, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.25">
@@ -6473,7 +6776,7 @@
         <v>241</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>164</v>
+        <v>342</v>
       </c>
       <c r="D79" s="3">
         <v>1</v>
@@ -6483,7 +6786,7 @@
       </c>
       <c r="H79" t="str">
         <f t="shared" si="4"/>
-        <v>Niple de 1/2"</v>
+        <v>Niple 1/2"</v>
       </c>
       <c r="I79" s="7" t="s">
         <v>266</v>
@@ -6504,7 +6807,7 @@
       </c>
       <c r="N79" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Niple de 1/2"', 1, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Niple 1/2"', 1, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.25">
@@ -6516,7 +6819,7 @@
         <v>249</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>174</v>
+        <v>344</v>
       </c>
       <c r="D80" s="3">
         <v>11</v>
@@ -6526,7 +6829,7 @@
       </c>
       <c r="H80" t="str">
         <f t="shared" si="4"/>
-        <v>Pegamento de PVC 1/16" azul</v>
+        <v>Pegamento PVC 1/16" azul</v>
       </c>
       <c r="I80" s="7" t="s">
         <v>266</v>
@@ -6547,7 +6850,7 @@
       </c>
       <c r="N80" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Pegamento de PVC 1/16" azul', 11, 'Activo', 0, 0, 7 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Pegamento PVC 1/16" azul', 11, 'Activo', 0, 0, 7 ) ; </v>
       </c>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.25">
@@ -6559,7 +6862,7 @@
         <v>249</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>173</v>
+        <v>345</v>
       </c>
       <c r="D81" s="3">
         <v>10</v>
@@ -6569,7 +6872,7 @@
       </c>
       <c r="H81" t="str">
         <f t="shared" si="4"/>
-        <v>Pegamento de PVC 1/16" dorado</v>
+        <v>Pegamento PVC 1/16" dorado</v>
       </c>
       <c r="I81" s="7" t="s">
         <v>266</v>
@@ -6590,7 +6893,7 @@
       </c>
       <c r="N81" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Pegamento de PVC 1/16" dorado', 10, 'Activo', 0, 0, 7 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Pegamento PVC 1/16" dorado', 10, 'Activo', 0, 0, 7 ) ; </v>
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.25">
@@ -6602,7 +6905,7 @@
         <v>249</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>176</v>
+        <v>346</v>
       </c>
       <c r="D82" s="3">
         <v>8</v>
@@ -6612,7 +6915,7 @@
       </c>
       <c r="H82" t="str">
         <f t="shared" si="4"/>
-        <v>Pegamento de PVC 1/32" azul</v>
+        <v>Pegamento PVC 1/32" azul</v>
       </c>
       <c r="I82" s="7" t="s">
         <v>266</v>
@@ -6633,7 +6936,7 @@
       </c>
       <c r="N82" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Pegamento de PVC 1/32" azul', 8, 'Activo', 0, 0, 7 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Pegamento PVC 1/32" azul', 8, 'Activo', 0, 0, 7 ) ; </v>
       </c>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.25">
@@ -6645,7 +6948,7 @@
         <v>249</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>175</v>
+        <v>347</v>
       </c>
       <c r="D83" s="3">
         <v>7</v>
@@ -6655,7 +6958,7 @@
       </c>
       <c r="H83" t="str">
         <f t="shared" si="4"/>
-        <v>Pegamento de PVC 1/32" dorado</v>
+        <v>Pegamento PVC 1/32" dorado</v>
       </c>
       <c r="I83" s="7" t="s">
         <v>266</v>
@@ -6676,7 +6979,7 @@
       </c>
       <c r="N83" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Pegamento de PVC 1/32" dorado', 7, 'Activo', 0, 0, 7 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Pegamento PVC 1/32" dorado', 7, 'Activo', 0, 0, 7 ) ; </v>
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.25">
@@ -6688,7 +6991,7 @@
         <v>249</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>170</v>
+        <v>348</v>
       </c>
       <c r="D84" s="3">
         <v>28</v>
@@ -6698,7 +7001,7 @@
       </c>
       <c r="H84" t="str">
         <f t="shared" si="4"/>
-        <v>Pegamento de PVC 1/4" dorado</v>
+        <v>Pegamento PVC 1/4" dorado</v>
       </c>
       <c r="I84" s="7" t="s">
         <v>266</v>
@@ -6719,7 +7022,7 @@
       </c>
       <c r="N84" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Pegamento de PVC 1/4" dorado', 28, 'Activo', 0, 0, 7 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Pegamento PVC 1/4" dorado', 28, 'Activo', 0, 0, 7 ) ; </v>
       </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.25">
@@ -6731,7 +7034,7 @@
         <v>249</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>172</v>
+        <v>349</v>
       </c>
       <c r="D85" s="3">
         <v>25</v>
@@ -6741,7 +7044,7 @@
       </c>
       <c r="H85" t="str">
         <f t="shared" si="4"/>
-        <v>Pegamento de PVC 1/8" azul</v>
+        <v>Pegamento PVC 1/8" azul</v>
       </c>
       <c r="I85" s="7" t="s">
         <v>266</v>
@@ -6762,7 +7065,7 @@
       </c>
       <c r="N85" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Pegamento de PVC 1/8" azul', 25, 'Activo', 0, 0, 7 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Pegamento PVC 1/8" azul', 25, 'Activo', 0, 0, 7 ) ; </v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.25">
@@ -6774,7 +7077,7 @@
         <v>249</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>171</v>
+        <v>350</v>
       </c>
       <c r="D86" s="3">
         <v>15</v>
@@ -6784,7 +7087,7 @@
       </c>
       <c r="H86" t="str">
         <f t="shared" si="4"/>
-        <v>Pegamento de PVC 1/8" dorado</v>
+        <v>Pegamento PVC 1/8" dorado</v>
       </c>
       <c r="I86" s="7" t="s">
         <v>266</v>
@@ -6805,7 +7108,7 @@
       </c>
       <c r="N86" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Pegamento de PVC 1/8" dorado', 15, 'Activo', 0, 0, 7 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Pegamento PVC 1/8" dorado', 15, 'Activo', 0, 0, 7 ) ; </v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
@@ -6817,7 +7120,7 @@
         <v>249</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>177</v>
+        <v>351</v>
       </c>
       <c r="D87" s="3">
         <v>6.5</v>
@@ -6827,7 +7130,7 @@
       </c>
       <c r="H87" t="str">
         <f t="shared" si="4"/>
-        <v>Pegamento de PVC agua caliente</v>
+        <v>Pegamento PVC agua caliente</v>
       </c>
       <c r="I87" s="7" t="s">
         <v>266</v>
@@ -6848,7 +7151,7 @@
       </c>
       <c r="N87" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Pegamento de PVC agua caliente', 6.5, 'Activo', 0, 0, 7 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Pegamento PVC agua caliente', 6.5, 'Activo', 0, 0, 7 ) ; </v>
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.25">
@@ -6860,7 +7163,7 @@
         <v>249</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>214</v>
+        <v>352</v>
       </c>
       <c r="D88" s="3">
         <v>14</v>
@@ -6870,7 +7173,7 @@
       </c>
       <c r="H88" t="str">
         <f t="shared" si="4"/>
-        <v>Pegamento en polvo - celima</v>
+        <v>Pegamento polvo - celima</v>
       </c>
       <c r="I88" s="7" t="s">
         <v>266</v>
@@ -6891,7 +7194,7 @@
       </c>
       <c r="N88" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Pegamento en polvo - celima', 14, 'Activo', 0, 0, 7 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Pegamento polvo - celima', 14, 'Activo', 0, 0, 7 ) ; </v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
@@ -7032,7 +7335,7 @@
         <v>241</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>156</v>
+        <v>353</v>
       </c>
       <c r="D92" s="3">
         <v>3.5</v>
@@ -7042,7 +7345,7 @@
       </c>
       <c r="H92" t="str">
         <f t="shared" si="4"/>
-        <v>Reduccion de desague 4" a 2"</v>
+        <v>Reduccion desague 4"a2"</v>
       </c>
       <c r="I92" s="7" t="s">
         <v>266</v>
@@ -7063,7 +7366,7 @@
       </c>
       <c r="N92" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Reduccion de desague 4" a 2"', 3.5, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Reduccion desague 4"a2"', 3.5, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.25">
@@ -7075,7 +7378,7 @@
         <v>241</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>218</v>
+        <v>354</v>
       </c>
       <c r="D93" s="3">
         <v>14</v>
@@ -7085,7 +7388,7 @@
       </c>
       <c r="H93" t="str">
         <f t="shared" si="4"/>
-        <v>Rodillo de 12" - toro</v>
+        <v>Rodillo 12" - toro</v>
       </c>
       <c r="I93" s="7" t="s">
         <v>266</v>
@@ -7106,7 +7409,7 @@
       </c>
       <c r="N93" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Rodillo de 12" - toro', 14, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Rodillo 12" - toro', 14, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
@@ -7118,7 +7421,7 @@
         <v>241</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>219</v>
+        <v>355</v>
       </c>
       <c r="D94" s="3">
         <v>12</v>
@@ -7128,7 +7431,7 @@
       </c>
       <c r="H94" t="str">
         <f t="shared" si="4"/>
-        <v>Rodillo de 9" - toro</v>
+        <v>Rodillo 9" - toro</v>
       </c>
       <c r="I94" s="7" t="s">
         <v>266</v>
@@ -7149,7 +7452,7 @@
       </c>
       <c r="N94" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Rodillo de 9" - toro', 12, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Rodillo 9" - toro', 12, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.25">
@@ -7161,7 +7464,7 @@
         <v>241</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>169</v>
+        <v>356</v>
       </c>
       <c r="D95" s="3">
         <v>5</v>
@@ -7171,7 +7474,7 @@
       </c>
       <c r="H95" t="str">
         <f t="shared" si="4"/>
-        <v>Tee bronce de 1/2"</v>
+        <v>Tee bronce 1/2"</v>
       </c>
       <c r="I95" s="7" t="s">
         <v>266</v>
@@ -7192,7 +7495,7 @@
       </c>
       <c r="N95" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Tee bronce de 1/2"', 5, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Tee bronce 1/2"', 5, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.25">
@@ -7204,7 +7507,7 @@
         <v>241</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>152</v>
+        <v>357</v>
       </c>
       <c r="D96" s="3">
         <v>1.5</v>
@@ -7214,7 +7517,7 @@
       </c>
       <c r="H96" t="str">
         <f t="shared" si="4"/>
-        <v>Tee de agua 1/2"</v>
+        <v>Tee agua 1/2"</v>
       </c>
       <c r="I96" s="7" t="s">
         <v>266</v>
@@ -7235,7 +7538,7 @@
       </c>
       <c r="N96" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Tee de agua 1/2"', 1.5, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Tee agua 1/2"', 1.5, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.25">
@@ -7247,7 +7550,7 @@
         <v>241</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>151</v>
+        <v>358</v>
       </c>
       <c r="D97" s="3">
         <v>3</v>
@@ -7257,7 +7560,7 @@
       </c>
       <c r="H97" t="str">
         <f t="shared" si="4"/>
-        <v>Tee de agua 3/4"</v>
+        <v>Tee agua 3/4"</v>
       </c>
       <c r="I97" s="7" t="s">
         <v>266</v>
@@ -7278,7 +7581,7 @@
       </c>
       <c r="N97" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Tee de agua 3/4"', 3, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Tee agua 3/4"', 3, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.25">
@@ -7290,7 +7593,7 @@
         <v>241</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>163</v>
+        <v>359</v>
       </c>
       <c r="D98" s="3">
         <v>1.5</v>
@@ -7300,7 +7603,7 @@
       </c>
       <c r="H98" t="str">
         <f t="shared" si="4"/>
-        <v>Tee de agua caliente 1/2"</v>
+        <v>Tee agua caliente 1/2"</v>
       </c>
       <c r="I98" s="7" t="s">
         <v>266</v>
@@ -7321,7 +7624,7 @@
       </c>
       <c r="N98" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Tee de agua caliente 1/2"', 1.5, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Tee agua caliente 1/2"', 1.5, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.25">
@@ -7333,7 +7636,7 @@
         <v>241</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>149</v>
+        <v>360</v>
       </c>
       <c r="D99" s="3">
         <v>6</v>
@@ -7343,7 +7646,7 @@
       </c>
       <c r="H99" t="str">
         <f t="shared" si="4"/>
-        <v>Tee de desague 4" x 2"</v>
+        <v>Tee desague 4" x 2"</v>
       </c>
       <c r="I99" s="7" t="s">
         <v>266</v>
@@ -7364,7 +7667,7 @@
       </c>
       <c r="N99" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Tee de desague 4" x 2"', 6, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Tee desague 4" x 2"', 6, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.25">
@@ -7376,7 +7679,7 @@
         <v>241</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>147</v>
+        <v>361</v>
       </c>
       <c r="D100" s="3">
         <v>7</v>
@@ -7386,7 +7689,7 @@
       </c>
       <c r="H100" t="str">
         <f t="shared" si="4"/>
-        <v>Tee de desague 4" x 4"</v>
+        <v>Tee desague 4" x 4"</v>
       </c>
       <c r="I100" s="7" t="s">
         <v>266</v>
@@ -7407,7 +7710,7 @@
       </c>
       <c r="N100" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Tee de desague 4" x 4"', 7, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Tee desague 4" x 4"', 7, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.25">
@@ -7419,7 +7722,7 @@
         <v>241</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>150</v>
+        <v>362</v>
       </c>
       <c r="D101" s="3">
         <v>3.5</v>
@@ -7429,7 +7732,7 @@
       </c>
       <c r="H101" t="str">
         <f t="shared" si="4"/>
-        <v>Tee de desague sanitaria 2"</v>
+        <v>Tee desague sanitaria 2"</v>
       </c>
       <c r="I101" s="7" t="s">
         <v>266</v>
@@ -7450,7 +7753,7 @@
       </c>
       <c r="N101" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Tee de desague sanitaria 2"', 3.5, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Tee desague sanitaria 2"', 3.5, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.25">
@@ -7505,7 +7808,7 @@
         <v>241</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>130</v>
+        <v>363</v>
       </c>
       <c r="D103" s="4">
         <v>10</v>
@@ -7515,7 +7818,7 @@
       </c>
       <c r="H103" t="str">
         <f t="shared" si="4"/>
-        <v>Tubo de agua 1/2"</v>
+        <v>Tubo agua 1/2"</v>
       </c>
       <c r="I103" s="7" t="s">
         <v>266</v>
@@ -7536,7 +7839,7 @@
       </c>
       <c r="N103" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Tubo de agua 1/2"', 10, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Tubo agua 1/2"', 10, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.25">
@@ -7548,7 +7851,7 @@
         <v>241</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>131</v>
+        <v>364</v>
       </c>
       <c r="D104" s="3">
         <v>18</v>
@@ -7558,7 +7861,7 @@
       </c>
       <c r="H104" t="str">
         <f t="shared" si="4"/>
-        <v>Tubo de agua 3/4"</v>
+        <v>Tubo agua 3/4"</v>
       </c>
       <c r="I104" s="7" t="s">
         <v>266</v>
@@ -7579,7 +7882,7 @@
       </c>
       <c r="N104" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Tubo de agua 3/4"', 18, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Tubo agua 3/4"', 18, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.25">
@@ -7591,7 +7894,7 @@
         <v>241</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>132</v>
+        <v>365</v>
       </c>
       <c r="D105" s="3">
         <v>18</v>
@@ -7601,7 +7904,7 @@
       </c>
       <c r="H105" t="str">
         <f t="shared" si="4"/>
-        <v>Tubo de agua caliente 1/2"</v>
+        <v>Tubo agua caliente 1/2"</v>
       </c>
       <c r="I105" s="7" t="s">
         <v>266</v>
@@ -7622,7 +7925,7 @@
       </c>
       <c r="N105" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Tubo de agua caliente 1/2"', 18, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Tubo agua caliente 1/2"', 18, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.25">
@@ -7634,7 +7937,7 @@
         <v>241</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>128</v>
+        <v>366</v>
       </c>
       <c r="D106" s="3">
         <v>10</v>
@@ -7644,7 +7947,7 @@
       </c>
       <c r="H106" t="str">
         <f t="shared" si="4"/>
-        <v>Tubo de agua desague 2"</v>
+        <v>Tubo desague 2"</v>
       </c>
       <c r="I106" s="7" t="s">
         <v>266</v>
@@ -7665,7 +7968,7 @@
       </c>
       <c r="N106" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Tubo de agua desague 2"', 10, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Tubo desague 2"', 10, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.25">
@@ -7677,7 +7980,7 @@
         <v>241</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>129</v>
+        <v>367</v>
       </c>
       <c r="D107" s="3">
         <v>17</v>
@@ -7687,7 +7990,7 @@
       </c>
       <c r="H107" t="str">
         <f t="shared" si="4"/>
-        <v>Tubo de agua desague 3"</v>
+        <v>Tubo desague 3"</v>
       </c>
       <c r="I107" s="7" t="s">
         <v>266</v>
@@ -7708,7 +8011,7 @@
       </c>
       <c r="N107" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Tubo de agua desague 3"', 17, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Tubo desague 3"', 17, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.25">
@@ -7720,7 +8023,7 @@
         <v>241</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>127</v>
+        <v>368</v>
       </c>
       <c r="D108" s="3">
         <v>20</v>
@@ -7730,7 +8033,7 @@
       </c>
       <c r="H108" t="str">
         <f t="shared" si="4"/>
-        <v>Tubo de agua desague 4"</v>
+        <v>Tubo desague 4"</v>
       </c>
       <c r="I108" s="7" t="s">
         <v>266</v>
@@ -7751,7 +8054,7 @@
       </c>
       <c r="N108" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Tubo de agua desague 4"', 20, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Tubo desague 4"', 20, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.25">
@@ -7763,7 +8066,7 @@
         <v>241</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>133</v>
+        <v>369</v>
       </c>
       <c r="D109" s="3">
         <v>6</v>
@@ -7773,7 +8076,7 @@
       </c>
       <c r="H109" t="str">
         <f t="shared" si="4"/>
-        <v>Tubo de luz 1"</v>
+        <v>Tubo luz 1"</v>
       </c>
       <c r="I109" s="7" t="s">
         <v>266</v>
@@ -7794,7 +8097,7 @@
       </c>
       <c r="N109" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Tubo de luz 1"', 6, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Tubo luz 1"', 6, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.25">
@@ -7806,7 +8109,7 @@
         <v>241</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>134</v>
+        <v>370</v>
       </c>
       <c r="D110" s="3">
         <v>3</v>
@@ -7816,7 +8119,7 @@
       </c>
       <c r="H110" t="str">
         <f t="shared" si="4"/>
-        <v>Tubo de luz 3/4"</v>
+        <v>Tubo luz 3/4"</v>
       </c>
       <c r="I110" s="7" t="s">
         <v>266</v>
@@ -7837,7 +8140,7 @@
       </c>
       <c r="N110" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Tubo de luz 3/4"', 3, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Tubo luz 3/4"', 3, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.25">
@@ -7849,7 +8152,7 @@
         <v>241</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>167</v>
+        <v>371</v>
       </c>
       <c r="D111" s="3">
         <v>4</v>
@@ -7859,7 +8162,7 @@
       </c>
       <c r="H111" t="str">
         <f t="shared" si="4"/>
-        <v>Union bronce de 1/2"</v>
+        <v>Union bronce 1/2"</v>
       </c>
       <c r="I111" s="7" t="s">
         <v>266</v>
@@ -7880,7 +8183,7 @@
       </c>
       <c r="N111" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Union bronce de 1/2"', 4, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Union bronce 1/2"', 4, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.25">
@@ -7892,7 +8195,7 @@
         <v>241</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>157</v>
+        <v>372</v>
       </c>
       <c r="D112" s="3">
         <v>1</v>
@@ -7902,7 +8205,7 @@
       </c>
       <c r="H112" t="str">
         <f t="shared" si="4"/>
-        <v>Union de agua 1/2"</v>
+        <v>Union agua 1/2"</v>
       </c>
       <c r="I112" s="7" t="s">
         <v>266</v>
@@ -7923,7 +8226,7 @@
       </c>
       <c r="N112" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Union de agua 1/2"', 1, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Union agua 1/2"', 1, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.25">
@@ -7935,7 +8238,7 @@
         <v>241</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>158</v>
+        <v>373</v>
       </c>
       <c r="D113" s="3">
         <v>2.5</v>
@@ -7945,7 +8248,7 @@
       </c>
       <c r="H113" t="str">
         <f t="shared" si="4"/>
-        <v>Union de agua 3/4"</v>
+        <v>Union agua 3/4"</v>
       </c>
       <c r="I113" s="7" t="s">
         <v>266</v>
@@ -7966,7 +8269,7 @@
       </c>
       <c r="N113" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Union de agua 3/4"', 2.5, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Union agua 3/4"', 2.5, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.25">
@@ -7978,7 +8281,7 @@
         <v>250</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>193</v>
+        <v>374</v>
       </c>
       <c r="D114" s="3">
         <v>3</v>
@@ -7988,7 +8291,7 @@
       </c>
       <c r="H114" t="str">
         <f t="shared" si="4"/>
-        <v>Visagra de 3" (par)</v>
+        <v>Visagra 3" (par)</v>
       </c>
       <c r="I114" s="7" t="s">
         <v>266</v>
@@ -8009,7 +8312,7 @@
       </c>
       <c r="N114" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Visagra de 3" (par)', 3, 'Activo', 0, 0, 9 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Visagra 3" (par)', 3, 'Activo', 0, 0, 9 ) ; </v>
       </c>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.25">
@@ -8021,7 +8324,7 @@
         <v>250</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>192</v>
+        <v>375</v>
       </c>
       <c r="D115" s="3">
         <v>3.5</v>
@@ -8031,7 +8334,7 @@
       </c>
       <c r="H115" t="str">
         <f t="shared" si="4"/>
-        <v>Visagra de 3" capuchino (par)</v>
+        <v>Visagra 3" - capuchino (par)</v>
       </c>
       <c r="I115" s="7" t="s">
         <v>266</v>
@@ -8052,7 +8355,7 @@
       </c>
       <c r="N115" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Visagra de 3" capuchino (par)', 3.5, 'Activo', 0, 0, 9 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Visagra 3" - capuchino (par)', 3.5, 'Activo', 0, 0, 9 ) ; </v>
       </c>
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.25">
@@ -8064,7 +8367,7 @@
         <v>241</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>155</v>
+        <v>376</v>
       </c>
       <c r="D116" s="3">
         <v>3</v>
@@ -8074,7 +8377,7 @@
       </c>
       <c r="H116" t="str">
         <f t="shared" si="4"/>
-        <v>Yee de desague 2"</v>
+        <v>Yee desague 2"</v>
       </c>
       <c r="I116" s="7" t="s">
         <v>266</v>
@@ -8095,7 +8398,7 @@
       </c>
       <c r="N116" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Yee de desague 2"', 3, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Yee desague 2"', 3, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.25">
@@ -8107,7 +8410,7 @@
         <v>241</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>154</v>
+        <v>379</v>
       </c>
       <c r="D117" s="3">
         <v>6</v>
@@ -8117,7 +8420,7 @@
       </c>
       <c r="H117" t="str">
         <f t="shared" si="4"/>
-        <v>Yee de desague 4" x 2"</v>
+        <v>Yee desague 4"x2"</v>
       </c>
       <c r="I117" s="7" t="s">
         <v>266</v>
@@ -8138,7 +8441,7 @@
       </c>
       <c r="N117" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Yee de desague 4" x 2"', 6, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Yee desague 4"x2"', 6, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="118" spans="1:14" x14ac:dyDescent="0.25">
@@ -8150,7 +8453,7 @@
         <v>241</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>153</v>
+        <v>380</v>
       </c>
       <c r="D118" s="3">
         <v>10</v>
@@ -8160,7 +8463,7 @@
       </c>
       <c r="H118" t="str">
         <f t="shared" si="4"/>
-        <v>Yee de desague 4" x 4"</v>
+        <v>Yee desague 4"x4"</v>
       </c>
       <c r="I118" s="7" t="s">
         <v>266</v>
@@ -8181,7 +8484,7 @@
       </c>
       <c r="N118" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Yee de desague 4" x 4"', 10, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Yee desague 4"x4"', 10, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.25">
@@ -8193,7 +8496,7 @@
         <v>241</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>136</v>
+        <v>377</v>
       </c>
       <c r="D119" s="3">
         <v>3.5</v>
@@ -8203,7 +8506,7 @@
       </c>
       <c r="H119" t="str">
         <f t="shared" si="4"/>
-        <v>Yee sanitario de 2"</v>
+        <v>Yee sanitario 2"</v>
       </c>
       <c r="I119" s="7" t="s">
         <v>266</v>
@@ -8224,7 +8527,7 @@
       </c>
       <c r="N119" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Yee sanitario de 2"', 3.5, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Yee sanitario 2"', 3.5, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.25">
@@ -8236,7 +8539,7 @@
         <v>241</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>135</v>
+        <v>378</v>
       </c>
       <c r="D120" s="3">
         <v>12</v>
@@ -8246,7 +8549,7 @@
       </c>
       <c r="H120" t="str">
         <f t="shared" si="4"/>
-        <v>Yee sanitario de 4"</v>
+        <v>Yee sanitario 4"</v>
       </c>
       <c r="I120" s="7" t="s">
         <v>266</v>
@@ -8267,7 +8570,7 @@
       </c>
       <c r="N120" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Yee sanitario de 4"', 12, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Yee sanitario 4"', 12, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="121" spans="1:14" x14ac:dyDescent="0.25">
@@ -8279,7 +8582,7 @@
         <v>241</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>148</v>
+        <v>381</v>
       </c>
       <c r="D121" s="3">
         <v>7</v>
@@ -8289,7 +8592,7 @@
       </c>
       <c r="H121" t="str">
         <f t="shared" si="4"/>
-        <v>Yee sanitario de 4" x 2"</v>
+        <v>Yee sanitario 4"x2"</v>
       </c>
       <c r="I121" s="7" t="s">
         <v>266</v>
@@ -8310,7 +8613,7 @@
       </c>
       <c r="N121" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Yee sanitario de 4" x 2"', 7, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Yee sanitario 4"x2"', 7, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="122" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -8322,7 +8625,7 @@
         <v>241</v>
       </c>
       <c r="C122" s="8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D122" s="9">
         <v>1.5</v>
@@ -8365,7 +8668,7 @@
         <v>241</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D123" s="3">
         <v>1.5</v>
@@ -8408,7 +8711,7 @@
         <v>241</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D124" s="3">
         <v>22</v>
@@ -8451,7 +8754,7 @@
         <v>249</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D125" s="3">
         <v>3.5</v>
@@ -8494,7 +8797,7 @@
         <v>241</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>282</v>
+        <v>382</v>
       </c>
       <c r="D126" s="3">
         <v>8</v>
@@ -8504,7 +8807,7 @@
       </c>
       <c r="H126" t="str">
         <f t="shared" ref="H126" si="24">C126</f>
-        <v>Parante 3 metros</v>
+        <v>Parante 3m</v>
       </c>
       <c r="I126" s="7" t="s">
         <v>266</v>
@@ -8525,7 +8828,7 @@
       </c>
       <c r="N126" t="str">
         <f t="shared" ref="N126" si="27">CONCATENATE(G126,H126,I126,J126,K126,L126,M126)</f>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Parante 3 metros', 8, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Parante 3m', 8, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.25">
@@ -8537,7 +8840,7 @@
         <v>241</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>284</v>
+        <v>383</v>
       </c>
       <c r="D127" s="3">
         <v>7</v>
@@ -8547,13 +8850,13 @@
       </c>
       <c r="H127" t="str">
         <f t="shared" ref="H127:H129" si="28">C127</f>
-        <v>Parante 2.5 metros</v>
+        <v>Parante 2.5m</v>
       </c>
       <c r="I127" s="7" t="s">
         <v>266</v>
       </c>
       <c r="J127" s="3">
-        <f t="shared" ref="J127:J129" si="29">D127</f>
+        <f t="shared" ref="J127:J130" si="29">D127</f>
         <v>7</v>
       </c>
       <c r="K127" t="s">
@@ -8568,7 +8871,7 @@
       </c>
       <c r="N127" t="str">
         <f t="shared" ref="N127:N129" si="31">CONCATENATE(G127,H127,I127,J127,K127,L127,M127)</f>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Parante 2.5 metros', 7, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Parante 2.5m', 7, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="128" spans="1:14" x14ac:dyDescent="0.25">
@@ -8580,7 +8883,7 @@
         <v>241</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>283</v>
+        <v>384</v>
       </c>
       <c r="D128" s="3">
         <v>4.5</v>
@@ -8590,7 +8893,7 @@
       </c>
       <c r="H128" t="str">
         <f t="shared" si="28"/>
-        <v>Liston 3 metros</v>
+        <v>Liston 3m</v>
       </c>
       <c r="I128" s="7" t="s">
         <v>266</v>
@@ -8611,7 +8914,7 @@
       </c>
       <c r="N128" t="str">
         <f t="shared" si="31"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Liston 3 metros', 4.5, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Liston 3m', 4.5, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.25">
@@ -8623,7 +8926,7 @@
         <v>241</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>285</v>
+        <v>385</v>
       </c>
       <c r="D129" s="3">
         <v>4</v>
@@ -8633,7 +8936,7 @@
       </c>
       <c r="H129" t="str">
         <f t="shared" si="28"/>
-        <v>Liston 2.5 metros</v>
+        <v>Liston 2.5m</v>
       </c>
       <c r="I129" s="7" t="s">
         <v>266</v>
@@ -8654,7 +8957,50 @@
       </c>
       <c r="N129" t="str">
         <f t="shared" si="31"/>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Liston 2.5 metros', 4, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Liston 2.5m', 4, 'Activo', 0, 0, 3 ) ; </v>
+      </c>
+    </row>
+    <row r="130" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <f>VLOOKUP(B130,'Maestra de unidades'!$B:$C,2,0)</f>
+        <v>3</v>
+      </c>
+      <c r="B130" t="s">
+        <v>241</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="D130" s="3">
+        <v>4</v>
+      </c>
+      <c r="G130" t="s">
+        <v>267</v>
+      </c>
+      <c r="H130" t="str">
+        <f t="shared" ref="H130" si="32">C130</f>
+        <v>Clavo 2"y1/2"</v>
+      </c>
+      <c r="I130" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="J130" s="3">
+        <f t="shared" ref="J130" si="33">D130</f>
+        <v>4</v>
+      </c>
+      <c r="K130" t="s">
+        <v>269</v>
+      </c>
+      <c r="L130">
+        <f t="shared" ref="L130" si="34">A130</f>
+        <v>3</v>
+      </c>
+      <c r="M130" t="s">
+        <v>268</v>
+      </c>
+      <c r="N130" t="str">
+        <f t="shared" ref="N130" si="35">CONCATENATE(G130,H130,I130,J130,K130,L130,M130)</f>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Clavo 2"y1/2"', 4, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nuevos precios y logo
</commit_message>
<xml_diff>
--- a/database/BD/backup/precios.xlsx
+++ b/database/BD/backup/precios.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1139" uniqueCount="401">
   <si>
     <t>Tubos</t>
   </si>
@@ -1190,6 +1190,48 @@
   </si>
   <si>
     <t>Clavo 2"y1/2"</t>
+  </si>
+  <si>
+    <t>Arena gruesa (Carretilla)</t>
+  </si>
+  <si>
+    <t>carretilla</t>
+  </si>
+  <si>
+    <t>Sumidero</t>
+  </si>
+  <si>
+    <t>Arena gruesa (bolsa)</t>
+  </si>
+  <si>
+    <t>Arena fina (bolsa)</t>
+  </si>
+  <si>
+    <t>Tanque 1100L</t>
+  </si>
+  <si>
+    <t>Cemento (kilo)</t>
+  </si>
+  <si>
+    <t>yeso (kilo)</t>
+  </si>
+  <si>
+    <t>Espor Lay</t>
+  </si>
+  <si>
+    <t>Tiner 1/2L</t>
+  </si>
+  <si>
+    <t>Tiner 1L</t>
+  </si>
+  <si>
+    <t>Sika</t>
+  </si>
+  <si>
+    <t>Tee desague 2"</t>
+  </si>
+  <si>
+    <t>Teflon</t>
   </si>
 </sst>
 </file>
@@ -3424,10 +3466,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N130"/>
+  <dimension ref="A1:N143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A130"/>
+    <sheetView tabSelected="1" topLeftCell="D142" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G142" sqref="G142:N143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8856,7 +8898,7 @@
         <v>266</v>
       </c>
       <c r="J127" s="3">
-        <f t="shared" ref="J127:J130" si="29">D127</f>
+        <f t="shared" ref="J127:J129" si="29">D127</f>
         <v>7</v>
       </c>
       <c r="K127" t="s">
@@ -8972,21 +9014,21 @@
         <v>386</v>
       </c>
       <c r="D130" s="3">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="G130" t="s">
         <v>267</v>
       </c>
       <c r="H130" t="str">
-        <f t="shared" ref="H130" si="32">C130</f>
+        <f t="shared" ref="H130:H131" si="32">C130</f>
         <v>Clavo 2"y1/2"</v>
       </c>
       <c r="I130" s="7" t="s">
         <v>266</v>
       </c>
       <c r="J130" s="3">
-        <f t="shared" ref="J130" si="33">D130</f>
-        <v>4</v>
+        <f t="shared" ref="J130:J131" si="33">D130</f>
+        <v>4.5</v>
       </c>
       <c r="K130" t="s">
         <v>269</v>
@@ -9000,7 +9042,566 @@
       </c>
       <c r="N130" t="str">
         <f t="shared" ref="N130" si="35">CONCATENATE(G130,H130,I130,J130,K130,L130,M130)</f>
-        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Clavo 2"y1/2"', 4, 'Activo', 0, 0, 3 ) ; </v>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Clavo 2"y1/2"', 4.5, 'Activo', 0, 0, 3 ) ; </v>
+      </c>
+    </row>
+    <row r="131" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <f>VLOOKUP(B131,'Maestra de unidades'!$B:$C,2,0)</f>
+        <v>13</v>
+      </c>
+      <c r="B131" t="s">
+        <v>388</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="D131" s="3">
+        <v>5</v>
+      </c>
+      <c r="G131" t="s">
+        <v>267</v>
+      </c>
+      <c r="H131" t="str">
+        <f t="shared" ref="H131:H132" si="36">C131</f>
+        <v>Arena gruesa (Carretilla)</v>
+      </c>
+      <c r="I131" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="J131" s="3">
+        <f t="shared" ref="J131:J132" si="37">D131</f>
+        <v>5</v>
+      </c>
+      <c r="K131" t="s">
+        <v>269</v>
+      </c>
+      <c r="L131">
+        <f t="shared" ref="L131" si="38">A131</f>
+        <v>13</v>
+      </c>
+      <c r="M131" t="s">
+        <v>268</v>
+      </c>
+      <c r="N131" t="str">
+        <f t="shared" ref="N131" si="39">CONCATENATE(G131,H131,I131,J131,K131,L131,M131)</f>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Arena gruesa (Carretilla)', 5, 'Activo', 0, 0, 13 ) ; </v>
+      </c>
+    </row>
+    <row r="132" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <f>VLOOKUP(B132,'Maestra de unidades'!$B:$C,2,0)</f>
+        <v>3</v>
+      </c>
+      <c r="B132" t="s">
+        <v>241</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="D132" s="3">
+        <v>4</v>
+      </c>
+      <c r="G132" t="s">
+        <v>267</v>
+      </c>
+      <c r="H132" t="str">
+        <f t="shared" ref="H132" si="40">C132</f>
+        <v>Sumidero</v>
+      </c>
+      <c r="I132" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="J132" s="3">
+        <f t="shared" ref="J132:J134" si="41">D132</f>
+        <v>4</v>
+      </c>
+      <c r="K132" t="s">
+        <v>269</v>
+      </c>
+      <c r="L132">
+        <f t="shared" ref="L132" si="42">A132</f>
+        <v>3</v>
+      </c>
+      <c r="M132" t="s">
+        <v>268</v>
+      </c>
+      <c r="N132" t="str">
+        <f t="shared" ref="N132" si="43">CONCATENATE(G132,H132,I132,J132,K132,L132,M132)</f>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Sumidero', 4, 'Activo', 0, 0, 3 ) ; </v>
+      </c>
+    </row>
+    <row r="133" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <f>VLOOKUP(B133,'Maestra de unidades'!$B:$C,2,0)</f>
+        <v>1</v>
+      </c>
+      <c r="B133" t="s">
+        <v>244</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="D133" s="3">
+        <v>3</v>
+      </c>
+      <c r="G133" t="s">
+        <v>267</v>
+      </c>
+      <c r="H133" t="str">
+        <f t="shared" ref="H133:H135" si="44">C133</f>
+        <v>Arena gruesa (bolsa)</v>
+      </c>
+      <c r="I133" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="J133" s="3">
+        <f t="shared" ref="J133:J134" si="45">D133</f>
+        <v>3</v>
+      </c>
+      <c r="K133" t="s">
+        <v>269</v>
+      </c>
+      <c r="L133">
+        <f t="shared" ref="L133:L134" si="46">A133</f>
+        <v>1</v>
+      </c>
+      <c r="M133" t="s">
+        <v>268</v>
+      </c>
+      <c r="N133" t="str">
+        <f t="shared" ref="N133:N134" si="47">CONCATENATE(G133,H133,I133,J133,K133,L133,M133)</f>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Arena gruesa (bolsa)', 3, 'Activo', 0, 0, 1 ) ; </v>
+      </c>
+    </row>
+    <row r="134" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <f>VLOOKUP(B134,'Maestra de unidades'!$B:$C,2,0)</f>
+        <v>1</v>
+      </c>
+      <c r="B134" t="s">
+        <v>244</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D134" s="3">
+        <v>3</v>
+      </c>
+      <c r="G134" t="s">
+        <v>267</v>
+      </c>
+      <c r="H134" t="str">
+        <f t="shared" si="44"/>
+        <v>Arena fina (bolsa)</v>
+      </c>
+      <c r="I134" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="J134" s="3">
+        <f t="shared" si="45"/>
+        <v>3</v>
+      </c>
+      <c r="K134" t="s">
+        <v>269</v>
+      </c>
+      <c r="L134">
+        <f t="shared" si="46"/>
+        <v>1</v>
+      </c>
+      <c r="M134" t="s">
+        <v>268</v>
+      </c>
+      <c r="N134" t="str">
+        <f t="shared" si="47"/>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Arena fina (bolsa)', 3, 'Activo', 0, 0, 1 ) ; </v>
+      </c>
+    </row>
+    <row r="135" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <f>VLOOKUP(B135,'Maestra de unidades'!$B:$C,2,0)</f>
+        <v>3</v>
+      </c>
+      <c r="B135" t="s">
+        <v>241</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="D135" s="3">
+        <v>410</v>
+      </c>
+      <c r="G135" t="s">
+        <v>267</v>
+      </c>
+      <c r="H135" t="str">
+        <f t="shared" ref="H135" si="48">C135</f>
+        <v>Tanque 1100L</v>
+      </c>
+      <c r="I135" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="J135" s="3">
+        <f t="shared" ref="J135:J136" si="49">D135</f>
+        <v>410</v>
+      </c>
+      <c r="K135" t="s">
+        <v>269</v>
+      </c>
+      <c r="L135">
+        <f t="shared" ref="L135" si="50">A135</f>
+        <v>3</v>
+      </c>
+      <c r="M135" t="s">
+        <v>268</v>
+      </c>
+      <c r="N135" t="str">
+        <f t="shared" ref="N135" si="51">CONCATENATE(G135,H135,I135,J135,K135,L135,M135)</f>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Tanque 1100L', 410, 'Activo', 0, 0, 3 ) ; </v>
+      </c>
+    </row>
+    <row r="136" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <f>VLOOKUP(B136,'Maestra de unidades'!$B:$C,2,0)</f>
+        <v>3</v>
+      </c>
+      <c r="B136" t="s">
+        <v>241</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="D136" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="G136" t="s">
+        <v>267</v>
+      </c>
+      <c r="H136" t="str">
+        <f t="shared" ref="H136:H138" si="52">C136</f>
+        <v>Espor Lay</v>
+      </c>
+      <c r="I136" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="J136" s="3">
+        <f t="shared" ref="J136" si="53">D136</f>
+        <v>2.5</v>
+      </c>
+      <c r="K136" t="s">
+        <v>269</v>
+      </c>
+      <c r="L136">
+        <f t="shared" ref="L136" si="54">A136</f>
+        <v>3</v>
+      </c>
+      <c r="M136" t="s">
+        <v>268</v>
+      </c>
+      <c r="N136" t="str">
+        <f t="shared" ref="N136" si="55">CONCATENATE(G136,H136,I136,J136,K136,L136,M136)</f>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Espor Lay', 2.5, 'Activo', 0, 0, 3 ) ; </v>
+      </c>
+    </row>
+    <row r="137" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <f>VLOOKUP(B137,'Maestra de unidades'!$B:$C,2,0)</f>
+        <v>6</v>
+      </c>
+      <c r="B137" t="s">
+        <v>242</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="D137" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="G137" t="s">
+        <v>267</v>
+      </c>
+      <c r="H137" t="str">
+        <f t="shared" ref="H137:H139" si="56">C137</f>
+        <v>Cemento (kilo)</v>
+      </c>
+      <c r="I137" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="J137" s="3">
+        <f t="shared" ref="J137:J140" si="57">D137</f>
+        <v>0.7</v>
+      </c>
+      <c r="K137" t="s">
+        <v>269</v>
+      </c>
+      <c r="L137">
+        <f t="shared" ref="L137:L138" si="58">A137</f>
+        <v>6</v>
+      </c>
+      <c r="M137" t="s">
+        <v>268</v>
+      </c>
+      <c r="N137" t="str">
+        <f t="shared" ref="N137:N138" si="59">CONCATENATE(G137,H137,I137,J137,K137,L137,M137)</f>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Cemento (kilo)', 0.7, 'Activo', 0, 0, 6 ) ; </v>
+      </c>
+    </row>
+    <row r="138" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <f>VLOOKUP(B138,'Maestra de unidades'!$B:$C,2,0)</f>
+        <v>6</v>
+      </c>
+      <c r="B138" t="s">
+        <v>242</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="D138" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="G138" t="s">
+        <v>267</v>
+      </c>
+      <c r="H138" t="str">
+        <f t="shared" si="56"/>
+        <v>yeso (kilo)</v>
+      </c>
+      <c r="I138" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="J138" s="3">
+        <f t="shared" si="57"/>
+        <v>0.7</v>
+      </c>
+      <c r="K138" t="s">
+        <v>269</v>
+      </c>
+      <c r="L138">
+        <f t="shared" si="58"/>
+        <v>6</v>
+      </c>
+      <c r="M138" t="s">
+        <v>268</v>
+      </c>
+      <c r="N138" t="str">
+        <f t="shared" si="59"/>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'yeso (kilo)', 0.7, 'Activo', 0, 0, 6 ) ; </v>
+      </c>
+    </row>
+    <row r="139" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <f>VLOOKUP(B139,'Maestra de unidades'!$B:$C,2,0)</f>
+        <v>7</v>
+      </c>
+      <c r="B139" t="s">
+        <v>249</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="D139" s="3">
+        <v>3</v>
+      </c>
+      <c r="G139" t="s">
+        <v>267</v>
+      </c>
+      <c r="H139" t="str">
+        <f t="shared" ref="H139:H141" si="60">C139</f>
+        <v>Tiner 1/2L</v>
+      </c>
+      <c r="I139" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="J139" s="3">
+        <f t="shared" ref="J139:J141" si="61">D139</f>
+        <v>3</v>
+      </c>
+      <c r="K139" t="s">
+        <v>269</v>
+      </c>
+      <c r="L139">
+        <f t="shared" ref="L139:L140" si="62">A139</f>
+        <v>7</v>
+      </c>
+      <c r="M139" t="s">
+        <v>268</v>
+      </c>
+      <c r="N139" t="str">
+        <f t="shared" ref="N139:N140" si="63">CONCATENATE(G139,H139,I139,J139,K139,L139,M139)</f>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Tiner 1/2L', 3, 'Activo', 0, 0, 7 ) ; </v>
+      </c>
+    </row>
+    <row r="140" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <f>VLOOKUP(B140,'Maestra de unidades'!$B:$C,2,0)</f>
+        <v>7</v>
+      </c>
+      <c r="B140" t="s">
+        <v>249</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="D140" s="3">
+        <v>6</v>
+      </c>
+      <c r="G140" t="s">
+        <v>267</v>
+      </c>
+      <c r="H140" t="str">
+        <f t="shared" si="60"/>
+        <v>Tiner 1L</v>
+      </c>
+      <c r="I140" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="J140" s="3">
+        <f t="shared" si="61"/>
+        <v>6</v>
+      </c>
+      <c r="K140" t="s">
+        <v>269</v>
+      </c>
+      <c r="L140">
+        <f t="shared" si="62"/>
+        <v>7</v>
+      </c>
+      <c r="M140" t="s">
+        <v>268</v>
+      </c>
+      <c r="N140" t="str">
+        <f t="shared" si="63"/>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Tiner 1L', 6, 'Activo', 0, 0, 7 ) ; </v>
+      </c>
+    </row>
+    <row r="141" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <f>VLOOKUP(B141,'Maestra de unidades'!$B:$C,2,0)</f>
+        <v>1</v>
+      </c>
+      <c r="B141" t="s">
+        <v>244</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="D141" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="G141" t="s">
+        <v>267</v>
+      </c>
+      <c r="H141" t="str">
+        <f t="shared" ref="H141:H142" si="64">C141</f>
+        <v>Sika</v>
+      </c>
+      <c r="I141" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="J141" s="3">
+        <f t="shared" ref="J141:J142" si="65">D141</f>
+        <v>4.5</v>
+      </c>
+      <c r="K141" t="s">
+        <v>269</v>
+      </c>
+      <c r="L141">
+        <f t="shared" ref="L141" si="66">A141</f>
+        <v>1</v>
+      </c>
+      <c r="M141" t="s">
+        <v>268</v>
+      </c>
+      <c r="N141" t="str">
+        <f t="shared" ref="N141" si="67">CONCATENATE(G141,H141,I141,J141,K141,L141,M141)</f>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Sika', 4.5, 'Activo', 0, 0, 1 ) ; </v>
+      </c>
+    </row>
+    <row r="142" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <f>VLOOKUP(B142,'Maestra de unidades'!$B:$C,2,0)</f>
+        <v>3</v>
+      </c>
+      <c r="B142" t="s">
+        <v>241</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="D142" s="3">
+        <v>3</v>
+      </c>
+      <c r="G142" t="s">
+        <v>267</v>
+      </c>
+      <c r="H142" t="str">
+        <f t="shared" ref="H142:H143" si="68">C142</f>
+        <v>Tee desague 2"</v>
+      </c>
+      <c r="I142" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="J142" s="3">
+        <f t="shared" ref="J142:J143" si="69">D142</f>
+        <v>3</v>
+      </c>
+      <c r="K142" t="s">
+        <v>269</v>
+      </c>
+      <c r="L142">
+        <f t="shared" ref="L142" si="70">A142</f>
+        <v>3</v>
+      </c>
+      <c r="M142" t="s">
+        <v>268</v>
+      </c>
+      <c r="N142" t="str">
+        <f t="shared" ref="N142" si="71">CONCATENATE(G142,H142,I142,J142,K142,L142,M142)</f>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Tee desague 2"', 3, 'Activo', 0, 0, 3 ) ; </v>
+      </c>
+    </row>
+    <row r="143" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <f>VLOOKUP(B143,'Maestra de unidades'!$B:$C,2,0)</f>
+        <v>3</v>
+      </c>
+      <c r="B143" t="s">
+        <v>241</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="D143" s="3">
+        <v>2</v>
+      </c>
+      <c r="G143" t="s">
+        <v>267</v>
+      </c>
+      <c r="H143" t="str">
+        <f t="shared" ref="H143" si="72">C143</f>
+        <v>Teflon</v>
+      </c>
+      <c r="I143" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="J143" s="3">
+        <f t="shared" ref="J143" si="73">D143</f>
+        <v>2</v>
+      </c>
+      <c r="K143" t="s">
+        <v>269</v>
+      </c>
+      <c r="L143">
+        <f t="shared" ref="L143" si="74">A143</f>
+        <v>3</v>
+      </c>
+      <c r="M143" t="s">
+        <v>268</v>
+      </c>
+      <c r="N143" t="str">
+        <f t="shared" ref="N143" si="75">CONCATENATE(G143,H143,I143,J143,K143,L143,M143)</f>
+        <v xml:space="preserve">INSERT INTO item ( name, price, state, realStock, availableStock, idUnit) VALUES ( 'Teflon', 2, 'Activo', 0, 0, 3 ) ; </v>
       </c>
     </row>
   </sheetData>
@@ -9013,10 +9614,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9161,6 +9762,17 @@
         <v>12</v>
       </c>
     </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>388</v>
+      </c>
+      <c r="C14">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>